<commit_message>
Change comment content: store model component label now #177.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="22980" windowHeight="10220" tabRatio="500"/>
+    <workbookView xWindow="1360" yWindow="500" windowWidth="22980" windowHeight="10220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -863,9 +863,6 @@
     <t>snmassacrossline</t>
   </si>
   <si>
-    <t>model component</t>
-  </si>
-  <si>
     <t>ocean</t>
   </si>
   <si>
@@ -873,13 +870,16 @@
   </si>
   <si>
     <t>seaIce</t>
+  </si>
+  <si>
+    <t>actual comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -891,6 +891,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -913,14 +929,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1198,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E193" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1210,8 +1230,8 @@
     <col min="4" max="4" width="60.6640625" customWidth="1"/>
     <col min="5" max="5" width="80.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="80.6640625" customWidth="1"/>
+    <col min="8" max="1024" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1234,7 +1254,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1242,13 +1262,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1256,13 +1276,13 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1270,13 +1290,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1284,13 +1304,13 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1298,13 +1318,13 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1312,13 +1332,13 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1326,13 +1346,13 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1340,13 +1360,13 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1354,13 +1374,13 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1368,13 +1388,13 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1382,13 +1402,13 @@
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1396,13 +1416,13 @@
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1410,13 +1430,13 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1424,13 +1444,13 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
@@ -1438,13 +1458,13 @@
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
@@ -1452,13 +1472,13 @@
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
@@ -1466,13 +1486,13 @@
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
@@ -1480,13 +1500,13 @@
         <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
@@ -1494,13 +1514,13 @@
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
@@ -1508,13 +1528,13 @@
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
@@ -1522,13 +1542,13 @@
         <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
@@ -1536,13 +1556,13 @@
         <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
@@ -1550,13 +1570,13 @@
         <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
@@ -1564,13 +1584,13 @@
         <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.2">
@@ -1578,13 +1598,13 @@
         <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
@@ -1592,13 +1612,13 @@
         <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.2">
@@ -1606,13 +1626,13 @@
         <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.2">
@@ -1620,13 +1640,13 @@
         <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
@@ -1634,13 +1654,13 @@
         <v>36</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
@@ -1648,13 +1668,13 @@
         <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
       </c>
       <c r="G32" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.2">
@@ -1662,13 +1682,13 @@
         <v>38</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.2">
@@ -1676,13 +1696,13 @@
         <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.2">
@@ -1690,13 +1710,13 @@
         <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.2">
@@ -1704,13 +1724,13 @@
         <v>41</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
@@ -1718,13 +1738,13 @@
         <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F37" t="s">
         <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.2">
@@ -1732,13 +1752,13 @@
         <v>43</v>
       </c>
       <c r="E38" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.2">
@@ -1746,13 +1766,13 @@
         <v>44</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.2">
@@ -1760,13 +1780,13 @@
         <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F40" t="s">
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
@@ -1774,13 +1794,13 @@
         <v>46</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F41" t="s">
         <v>8</v>
       </c>
       <c r="G41" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
@@ -1788,13 +1808,13 @@
         <v>47</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
       </c>
       <c r="G42" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
@@ -1802,13 +1822,13 @@
         <v>48</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F43" t="s">
         <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
@@ -1816,13 +1836,13 @@
         <v>49</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F44" t="s">
         <v>8</v>
       </c>
       <c r="G44" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.2">
@@ -1830,13 +1850,13 @@
         <v>50</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F45" t="s">
         <v>8</v>
       </c>
       <c r="G45" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.2">
@@ -1844,13 +1864,13 @@
         <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F46" t="s">
         <v>8</v>
       </c>
       <c r="G46" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
@@ -1858,13 +1878,13 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F47" t="s">
         <v>8</v>
       </c>
       <c r="G47" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.2">
@@ -1872,13 +1892,13 @@
         <v>53</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F48" t="s">
         <v>8</v>
       </c>
       <c r="G48" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.2">
@@ -1886,13 +1906,13 @@
         <v>54</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F49" t="s">
         <v>8</v>
       </c>
       <c r="G49" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.2">
@@ -1900,13 +1920,13 @@
         <v>55</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F50" t="s">
         <v>8</v>
       </c>
       <c r="G50" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.2">
@@ -1914,13 +1934,13 @@
         <v>56</v>
       </c>
       <c r="E51" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F51" t="s">
         <v>8</v>
       </c>
       <c r="G51" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.2">
@@ -1928,13 +1948,13 @@
         <v>57</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F52" t="s">
         <v>8</v>
       </c>
       <c r="G52" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.2">
@@ -1942,13 +1962,13 @@
         <v>58</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F53" t="s">
         <v>8</v>
       </c>
       <c r="G53" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.2">
@@ -1956,13 +1976,13 @@
         <v>59</v>
       </c>
       <c r="E54" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F54" t="s">
         <v>8</v>
       </c>
       <c r="G54" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.2">
@@ -1970,13 +1990,13 @@
         <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F55" t="s">
         <v>8</v>
       </c>
       <c r="G55" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.2">
@@ -1984,13 +2004,13 @@
         <v>61</v>
       </c>
       <c r="E56" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.2">
@@ -1998,13 +2018,13 @@
         <v>62</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F57" t="s">
         <v>8</v>
       </c>
       <c r="G57" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.2">
@@ -2012,13 +2032,13 @@
         <v>63</v>
       </c>
       <c r="E58" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F58" t="s">
         <v>8</v>
       </c>
       <c r="G58" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.2">
@@ -2026,13 +2046,13 @@
         <v>64</v>
       </c>
       <c r="E59" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F59" t="s">
         <v>8</v>
       </c>
       <c r="G59" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.2">
@@ -2040,13 +2060,13 @@
         <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F60" t="s">
         <v>8</v>
       </c>
       <c r="G60" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.2">
@@ -2054,13 +2074,13 @@
         <v>66</v>
       </c>
       <c r="E61" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F61" t="s">
         <v>8</v>
       </c>
       <c r="G61" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.2">
@@ -2068,13 +2088,13 @@
         <v>67</v>
       </c>
       <c r="E62" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F62" t="s">
         <v>8</v>
       </c>
       <c r="G62" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.2">
@@ -2082,13 +2102,13 @@
         <v>68</v>
       </c>
       <c r="E63" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F63" t="s">
         <v>8</v>
       </c>
       <c r="G63" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.2">
@@ -2096,13 +2116,13 @@
         <v>69</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F64" t="s">
         <v>8</v>
       </c>
       <c r="G64" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.2">
@@ -2110,13 +2130,13 @@
         <v>70</v>
       </c>
       <c r="E65" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F65" t="s">
         <v>8</v>
       </c>
       <c r="G65" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.2">
@@ -2124,13 +2144,13 @@
         <v>71</v>
       </c>
       <c r="E66" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F66" t="s">
         <v>8</v>
       </c>
       <c r="G66" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.2">
@@ -2138,13 +2158,13 @@
         <v>72</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F67" t="s">
         <v>8</v>
       </c>
       <c r="G67" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.2">
@@ -2152,13 +2172,13 @@
         <v>73</v>
       </c>
       <c r="E68" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F68" t="s">
         <v>8</v>
       </c>
       <c r="G68" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.2">
@@ -2166,13 +2186,13 @@
         <v>74</v>
       </c>
       <c r="E69" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F69" t="s">
         <v>8</v>
       </c>
       <c r="G69" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.2">
@@ -2180,13 +2200,13 @@
         <v>75</v>
       </c>
       <c r="E70" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F70" t="s">
         <v>8</v>
       </c>
       <c r="G70" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.2">
@@ -2194,13 +2214,13 @@
         <v>76</v>
       </c>
       <c r="E71" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F71" t="s">
         <v>8</v>
       </c>
       <c r="G71" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.2">
@@ -2208,13 +2228,13 @@
         <v>77</v>
       </c>
       <c r="E72" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F72" t="s">
         <v>8</v>
       </c>
       <c r="G72" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.2">
@@ -2222,13 +2242,13 @@
         <v>78</v>
       </c>
       <c r="E73" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F73" t="s">
         <v>8</v>
       </c>
       <c r="G73" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.2">
@@ -2236,13 +2256,13 @@
         <v>79</v>
       </c>
       <c r="E74" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F74" t="s">
         <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.2">
@@ -2250,13 +2270,13 @@
         <v>80</v>
       </c>
       <c r="E75" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F75" t="s">
         <v>8</v>
       </c>
       <c r="G75" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.2">
@@ -2264,13 +2284,13 @@
         <v>81</v>
       </c>
       <c r="E76" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F76" t="s">
         <v>8</v>
       </c>
       <c r="G76" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.2">
@@ -2278,13 +2298,13 @@
         <v>82</v>
       </c>
       <c r="E77" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F77" t="s">
         <v>8</v>
       </c>
       <c r="G77" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.2">
@@ -2292,13 +2312,13 @@
         <v>83</v>
       </c>
       <c r="E78" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F78" t="s">
         <v>8</v>
       </c>
       <c r="G78" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.2">
@@ -2306,13 +2326,13 @@
         <v>84</v>
       </c>
       <c r="E79" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F79" t="s">
         <v>8</v>
       </c>
       <c r="G79" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.2">
@@ -2320,13 +2340,13 @@
         <v>85</v>
       </c>
       <c r="E80" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F80" t="s">
         <v>8</v>
       </c>
       <c r="G80" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.2">
@@ -2334,13 +2354,13 @@
         <v>86</v>
       </c>
       <c r="E81" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F81" t="s">
         <v>8</v>
       </c>
       <c r="G81" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.2">
@@ -2348,13 +2368,13 @@
         <v>87</v>
       </c>
       <c r="E82" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F82" t="s">
         <v>8</v>
       </c>
       <c r="G82" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.2">
@@ -2362,13 +2382,13 @@
         <v>88</v>
       </c>
       <c r="E83" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F83" t="s">
         <v>8</v>
       </c>
       <c r="G83" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.2">
@@ -2376,13 +2396,13 @@
         <v>89</v>
       </c>
       <c r="E84" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F84" t="s">
         <v>8</v>
       </c>
       <c r="G84" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.2">
@@ -2390,13 +2410,13 @@
         <v>90</v>
       </c>
       <c r="E85" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F85" t="s">
         <v>8</v>
       </c>
       <c r="G85" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.2">
@@ -2404,13 +2424,13 @@
         <v>91</v>
       </c>
       <c r="E86" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F86" t="s">
         <v>8</v>
       </c>
       <c r="G86" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.2">
@@ -2418,13 +2438,13 @@
         <v>92</v>
       </c>
       <c r="E87" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F87" t="s">
         <v>8</v>
       </c>
       <c r="G87" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.2">
@@ -2432,13 +2452,13 @@
         <v>93</v>
       </c>
       <c r="E88" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F88" t="s">
         <v>8</v>
       </c>
       <c r="G88" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.2">
@@ -2446,13 +2466,13 @@
         <v>94</v>
       </c>
       <c r="E89" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F89" t="s">
         <v>8</v>
       </c>
       <c r="G89" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.2">
@@ -2460,13 +2480,13 @@
         <v>95</v>
       </c>
       <c r="E90" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F90" t="s">
         <v>8</v>
       </c>
       <c r="G90" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.2">
@@ -2474,13 +2494,13 @@
         <v>96</v>
       </c>
       <c r="E91" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F91" t="s">
         <v>8</v>
       </c>
       <c r="G91" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.2">
@@ -2488,13 +2508,13 @@
         <v>97</v>
       </c>
       <c r="E92" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F92" t="s">
         <v>8</v>
       </c>
       <c r="G92" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.2">
@@ -2502,13 +2522,13 @@
         <v>98</v>
       </c>
       <c r="E93" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F93" t="s">
         <v>8</v>
       </c>
       <c r="G93" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.2">
@@ -2516,13 +2536,13 @@
         <v>99</v>
       </c>
       <c r="E94" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F94" t="s">
         <v>8</v>
       </c>
       <c r="G94" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.2">
@@ -2530,13 +2550,13 @@
         <v>100</v>
       </c>
       <c r="E95" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F95" t="s">
         <v>8</v>
       </c>
       <c r="G95" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.2">
@@ -2544,13 +2564,13 @@
         <v>101</v>
       </c>
       <c r="E96" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F96" t="s">
         <v>8</v>
       </c>
       <c r="G96" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.2">
@@ -2558,13 +2578,13 @@
         <v>102</v>
       </c>
       <c r="E97" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F97" t="s">
         <v>8</v>
       </c>
       <c r="G97" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.2">
@@ -2572,13 +2592,13 @@
         <v>103</v>
       </c>
       <c r="E98" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F98" t="s">
         <v>8</v>
       </c>
       <c r="G98" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.2">
@@ -2586,13 +2606,13 @@
         <v>104</v>
       </c>
       <c r="E99" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F99" t="s">
         <v>8</v>
       </c>
       <c r="G99" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.2">
@@ -2600,13 +2620,13 @@
         <v>105</v>
       </c>
       <c r="E100" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F100" t="s">
         <v>8</v>
       </c>
       <c r="G100" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.2">
@@ -2614,13 +2634,13 @@
         <v>106</v>
       </c>
       <c r="E101" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F101" t="s">
         <v>8</v>
       </c>
       <c r="G101" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.2">
@@ -2628,13 +2648,13 @@
         <v>107</v>
       </c>
       <c r="E102" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F102" t="s">
         <v>8</v>
       </c>
       <c r="G102" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.2">
@@ -2642,13 +2662,13 @@
         <v>108</v>
       </c>
       <c r="E103" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F103" t="s">
         <v>8</v>
       </c>
       <c r="G103" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.2">
@@ -2656,13 +2676,13 @@
         <v>109</v>
       </c>
       <c r="E104" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F104" t="s">
         <v>8</v>
       </c>
       <c r="G104" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.2">
@@ -2670,13 +2690,13 @@
         <v>110</v>
       </c>
       <c r="E105" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F105" t="s">
         <v>8</v>
       </c>
       <c r="G105" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.2">
@@ -2684,13 +2704,13 @@
         <v>111</v>
       </c>
       <c r="E106" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F106" t="s">
         <v>8</v>
       </c>
       <c r="G106" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.2">
@@ -2698,13 +2718,13 @@
         <v>112</v>
       </c>
       <c r="E107" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F107" t="s">
         <v>8</v>
       </c>
       <c r="G107" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.2">
@@ -2712,13 +2732,13 @@
         <v>113</v>
       </c>
       <c r="E108" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="F108" t="s">
         <v>8</v>
       </c>
       <c r="G108" t="s">
-        <v>278</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.2">
@@ -2726,13 +2746,13 @@
         <v>114</v>
       </c>
       <c r="E109" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F109" t="s">
         <v>8</v>
       </c>
       <c r="G109" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.2">
@@ -2740,13 +2760,13 @@
         <v>116</v>
       </c>
       <c r="E110" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F110" t="s">
         <v>8</v>
       </c>
       <c r="G110" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.2">
@@ -2754,13 +2774,13 @@
         <v>117</v>
       </c>
       <c r="E111" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F111" t="s">
         <v>8</v>
       </c>
       <c r="G111" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.2">
@@ -2768,13 +2788,13 @@
         <v>118</v>
       </c>
       <c r="E112" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F112" t="s">
         <v>8</v>
       </c>
       <c r="G112" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="113" spans="3:7" x14ac:dyDescent="0.2">
@@ -2782,13 +2802,13 @@
         <v>119</v>
       </c>
       <c r="E113" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F113" t="s">
         <v>8</v>
       </c>
       <c r="G113" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="3:7" x14ac:dyDescent="0.2">
@@ -2796,13 +2816,13 @@
         <v>120</v>
       </c>
       <c r="E114" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F114" t="s">
         <v>8</v>
       </c>
       <c r="G114" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.2">
@@ -2810,13 +2830,13 @@
         <v>121</v>
       </c>
       <c r="E115" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F115" t="s">
         <v>8</v>
       </c>
       <c r="G115" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.2">
@@ -2824,13 +2844,13 @@
         <v>122</v>
       </c>
       <c r="E116" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F116" t="s">
         <v>8</v>
       </c>
       <c r="G116" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.2">
@@ -2838,13 +2858,13 @@
         <v>123</v>
       </c>
       <c r="E117" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F117" t="s">
         <v>8</v>
       </c>
       <c r="G117" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.2">
@@ -2852,13 +2872,13 @@
         <v>124</v>
       </c>
       <c r="E118" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F118" t="s">
         <v>8</v>
       </c>
       <c r="G118" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.2">
@@ -2866,13 +2886,13 @@
         <v>125</v>
       </c>
       <c r="E119" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F119" t="s">
         <v>8</v>
       </c>
       <c r="G119" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.2">
@@ -2880,13 +2900,13 @@
         <v>126</v>
       </c>
       <c r="E120" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F120" t="s">
         <v>8</v>
       </c>
       <c r="G120" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="3:7" x14ac:dyDescent="0.2">
@@ -2894,13 +2914,13 @@
         <v>127</v>
       </c>
       <c r="E121" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F121" t="s">
         <v>8</v>
       </c>
       <c r="G121" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.2">
@@ -2908,13 +2928,13 @@
         <v>128</v>
       </c>
       <c r="E122" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F122" t="s">
         <v>8</v>
       </c>
       <c r="G122" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.2">
@@ -2922,13 +2942,13 @@
         <v>129</v>
       </c>
       <c r="E123" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F123" t="s">
         <v>8</v>
       </c>
       <c r="G123" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.2">
@@ -2936,13 +2956,13 @@
         <v>130</v>
       </c>
       <c r="E124" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F124" t="s">
         <v>8</v>
       </c>
       <c r="G124" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.2">
@@ -2950,13 +2970,13 @@
         <v>131</v>
       </c>
       <c r="E125" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F125" t="s">
         <v>8</v>
       </c>
       <c r="G125" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.2">
@@ -2964,13 +2984,13 @@
         <v>132</v>
       </c>
       <c r="E126" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F126" t="s">
         <v>8</v>
       </c>
       <c r="G126" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.2">
@@ -2978,13 +2998,13 @@
         <v>133</v>
       </c>
       <c r="E127" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F127" t="s">
         <v>8</v>
       </c>
       <c r="G127" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.2">
@@ -2992,13 +3012,13 @@
         <v>134</v>
       </c>
       <c r="E128" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F128" t="s">
         <v>8</v>
       </c>
       <c r="G128" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="129" spans="3:7" x14ac:dyDescent="0.2">
@@ -3006,13 +3026,13 @@
         <v>135</v>
       </c>
       <c r="E129" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F129" t="s">
         <v>8</v>
       </c>
       <c r="G129" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.2">
@@ -3020,13 +3040,13 @@
         <v>136</v>
       </c>
       <c r="E130" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F130" t="s">
         <v>8</v>
       </c>
       <c r="G130" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.2">
@@ -3034,13 +3054,13 @@
         <v>137</v>
       </c>
       <c r="E131" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F131" t="s">
         <v>8</v>
       </c>
       <c r="G131" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.2">
@@ -3048,13 +3068,13 @@
         <v>138</v>
       </c>
       <c r="E132" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F132" t="s">
         <v>8</v>
       </c>
       <c r="G132" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.2">
@@ -3062,13 +3082,13 @@
         <v>139</v>
       </c>
       <c r="E133" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F133" t="s">
         <v>8</v>
       </c>
       <c r="G133" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="134" spans="3:7" x14ac:dyDescent="0.2">
@@ -3076,13 +3096,13 @@
         <v>140</v>
       </c>
       <c r="E134" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F134" t="s">
         <v>8</v>
       </c>
       <c r="G134" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="3:7" x14ac:dyDescent="0.2">
@@ -3090,13 +3110,13 @@
         <v>141</v>
       </c>
       <c r="E135" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F135" t="s">
         <v>8</v>
       </c>
       <c r="G135" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="3:7" x14ac:dyDescent="0.2">
@@ -3104,13 +3124,13 @@
         <v>142</v>
       </c>
       <c r="E136" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F136" t="s">
         <v>8</v>
       </c>
       <c r="G136" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="137" spans="3:7" x14ac:dyDescent="0.2">
@@ -3118,13 +3138,13 @@
         <v>143</v>
       </c>
       <c r="E137" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F137" t="s">
         <v>8</v>
       </c>
       <c r="G137" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.2">
@@ -3132,13 +3152,13 @@
         <v>144</v>
       </c>
       <c r="E138" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F138" t="s">
         <v>8</v>
       </c>
       <c r="G138" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="139" spans="3:7" x14ac:dyDescent="0.2">
@@ -3146,13 +3166,13 @@
         <v>145</v>
       </c>
       <c r="E139" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F139" t="s">
         <v>8</v>
       </c>
       <c r="G139" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="140" spans="3:7" x14ac:dyDescent="0.2">
@@ -3160,13 +3180,13 @@
         <v>146</v>
       </c>
       <c r="E140" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F140" t="s">
         <v>8</v>
       </c>
       <c r="G140" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.2">
@@ -3174,13 +3194,13 @@
         <v>147</v>
       </c>
       <c r="E141" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F141" t="s">
         <v>8</v>
       </c>
       <c r="G141" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="142" spans="3:7" x14ac:dyDescent="0.2">
@@ -3188,13 +3208,13 @@
         <v>148</v>
       </c>
       <c r="E142" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F142" t="s">
         <v>8</v>
       </c>
       <c r="G142" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="143" spans="3:7" x14ac:dyDescent="0.2">
@@ -3202,13 +3222,13 @@
         <v>149</v>
       </c>
       <c r="E143" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F143" t="s">
         <v>8</v>
       </c>
       <c r="G143" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="144" spans="3:7" x14ac:dyDescent="0.2">
@@ -3216,13 +3236,13 @@
         <v>150</v>
       </c>
       <c r="E144" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F144" t="s">
         <v>8</v>
       </c>
       <c r="G144" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="145" spans="3:7" x14ac:dyDescent="0.2">
@@ -3230,13 +3250,13 @@
         <v>151</v>
       </c>
       <c r="E145" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F145" t="s">
         <v>8</v>
       </c>
       <c r="G145" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="146" spans="3:7" x14ac:dyDescent="0.2">
@@ -3244,13 +3264,13 @@
         <v>152</v>
       </c>
       <c r="E146" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F146" t="s">
         <v>8</v>
       </c>
       <c r="G146" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="147" spans="3:7" x14ac:dyDescent="0.2">
@@ -3258,13 +3278,13 @@
         <v>153</v>
       </c>
       <c r="E147" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F147" t="s">
         <v>8</v>
       </c>
       <c r="G147" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="148" spans="3:7" x14ac:dyDescent="0.2">
@@ -3272,13 +3292,13 @@
         <v>154</v>
       </c>
       <c r="E148" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F148" t="s">
         <v>8</v>
       </c>
       <c r="G148" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="149" spans="3:7" x14ac:dyDescent="0.2">
@@ -3286,13 +3306,13 @@
         <v>155</v>
       </c>
       <c r="E149" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F149" t="s">
         <v>8</v>
       </c>
       <c r="G149" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="150" spans="3:7" x14ac:dyDescent="0.2">
@@ -3300,13 +3320,13 @@
         <v>156</v>
       </c>
       <c r="E150" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F150" t="s">
         <v>8</v>
       </c>
       <c r="G150" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="151" spans="3:7" x14ac:dyDescent="0.2">
@@ -3314,13 +3334,13 @@
         <v>157</v>
       </c>
       <c r="E151" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F151" t="s">
         <v>8</v>
       </c>
       <c r="G151" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.2">
@@ -3328,13 +3348,13 @@
         <v>158</v>
       </c>
       <c r="E152" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F152" t="s">
         <v>8</v>
       </c>
       <c r="G152" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.2">
@@ -3342,13 +3362,13 @@
         <v>159</v>
       </c>
       <c r="E153" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F153" t="s">
         <v>8</v>
       </c>
       <c r="G153" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="154" spans="3:7" x14ac:dyDescent="0.2">
@@ -3356,13 +3376,13 @@
         <v>160</v>
       </c>
       <c r="E154" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F154" t="s">
         <v>8</v>
       </c>
       <c r="G154" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="155" spans="3:7" x14ac:dyDescent="0.2">
@@ -3370,13 +3390,13 @@
         <v>161</v>
       </c>
       <c r="E155" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F155" t="s">
         <v>8</v>
       </c>
       <c r="G155" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="3:7" x14ac:dyDescent="0.2">
@@ -3384,13 +3404,13 @@
         <v>162</v>
       </c>
       <c r="E156" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F156" t="s">
         <v>8</v>
       </c>
       <c r="G156" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="157" spans="3:7" x14ac:dyDescent="0.2">
@@ -3398,13 +3418,13 @@
         <v>163</v>
       </c>
       <c r="E157" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F157" t="s">
         <v>8</v>
       </c>
       <c r="G157" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="158" spans="3:7" x14ac:dyDescent="0.2">
@@ -3412,13 +3432,13 @@
         <v>164</v>
       </c>
       <c r="E158" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F158" t="s">
         <v>8</v>
       </c>
       <c r="G158" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="159" spans="3:7" x14ac:dyDescent="0.2">
@@ -3426,13 +3446,13 @@
         <v>165</v>
       </c>
       <c r="E159" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F159" t="s">
         <v>8</v>
       </c>
       <c r="G159" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="3:7" x14ac:dyDescent="0.2">
@@ -3440,13 +3460,13 @@
         <v>166</v>
       </c>
       <c r="E160" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F160" t="s">
         <v>8</v>
       </c>
       <c r="G160" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="161" spans="3:7" x14ac:dyDescent="0.2">
@@ -3454,13 +3474,13 @@
         <v>167</v>
       </c>
       <c r="E161" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F161" t="s">
         <v>8</v>
       </c>
       <c r="G161" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="162" spans="3:7" x14ac:dyDescent="0.2">
@@ -3468,13 +3488,13 @@
         <v>168</v>
       </c>
       <c r="E162" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F162" t="s">
         <v>8</v>
       </c>
       <c r="G162" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="3:7" x14ac:dyDescent="0.2">
@@ -3482,13 +3502,13 @@
         <v>169</v>
       </c>
       <c r="E163" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F163" t="s">
         <v>8</v>
       </c>
       <c r="G163" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="164" spans="3:7" x14ac:dyDescent="0.2">
@@ -3496,13 +3516,13 @@
         <v>170</v>
       </c>
       <c r="E164" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F164" t="s">
         <v>8</v>
       </c>
       <c r="G164" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.2">
@@ -3510,13 +3530,13 @@
         <v>171</v>
       </c>
       <c r="E165" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F165" t="s">
         <v>8</v>
       </c>
       <c r="G165" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.2">
@@ -3524,13 +3544,13 @@
         <v>172</v>
       </c>
       <c r="E166" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F166" t="s">
         <v>8</v>
       </c>
       <c r="G166" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="167" spans="3:7" x14ac:dyDescent="0.2">
@@ -3538,13 +3558,13 @@
         <v>173</v>
       </c>
       <c r="E167" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F167" t="s">
         <v>8</v>
       </c>
       <c r="G167" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.2">
@@ -3552,13 +3572,13 @@
         <v>174</v>
       </c>
       <c r="E168" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F168" t="s">
         <v>8</v>
       </c>
       <c r="G168" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="169" spans="3:7" x14ac:dyDescent="0.2">
@@ -3566,13 +3586,13 @@
         <v>175</v>
       </c>
       <c r="E169" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F169" t="s">
         <v>8</v>
       </c>
       <c r="G169" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="170" spans="3:7" x14ac:dyDescent="0.2">
@@ -3580,13 +3600,13 @@
         <v>176</v>
       </c>
       <c r="E170" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F170" t="s">
         <v>8</v>
       </c>
       <c r="G170" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="171" spans="3:7" x14ac:dyDescent="0.2">
@@ -3594,13 +3614,13 @@
         <v>177</v>
       </c>
       <c r="E171" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F171" t="s">
         <v>8</v>
       </c>
       <c r="G171" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="172" spans="3:7" x14ac:dyDescent="0.2">
@@ -3608,13 +3628,13 @@
         <v>178</v>
       </c>
       <c r="E172" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F172" t="s">
         <v>8</v>
       </c>
       <c r="G172" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="173" spans="3:7" x14ac:dyDescent="0.2">
@@ -3622,13 +3642,13 @@
         <v>179</v>
       </c>
       <c r="E173" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F173" t="s">
         <v>8</v>
       </c>
       <c r="G173" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.2">
@@ -3636,13 +3656,13 @@
         <v>180</v>
       </c>
       <c r="E174" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F174" t="s">
         <v>8</v>
       </c>
       <c r="G174" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="175" spans="3:7" x14ac:dyDescent="0.2">
@@ -3650,13 +3670,13 @@
         <v>181</v>
       </c>
       <c r="E175" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F175" t="s">
         <v>8</v>
       </c>
       <c r="G175" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="176" spans="3:7" x14ac:dyDescent="0.2">
@@ -3664,13 +3684,13 @@
         <v>182</v>
       </c>
       <c r="E176" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F176" t="s">
         <v>8</v>
       </c>
       <c r="G176" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="177" spans="3:7" x14ac:dyDescent="0.2">
@@ -3678,13 +3698,13 @@
         <v>183</v>
       </c>
       <c r="E177" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F177" t="s">
         <v>8</v>
       </c>
       <c r="G177" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="178" spans="3:7" x14ac:dyDescent="0.2">
@@ -3692,13 +3712,13 @@
         <v>184</v>
       </c>
       <c r="E178" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F178" t="s">
         <v>8</v>
       </c>
       <c r="G178" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="179" spans="3:7" x14ac:dyDescent="0.2">
@@ -3706,13 +3726,13 @@
         <v>185</v>
       </c>
       <c r="E179" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F179" t="s">
         <v>8</v>
       </c>
       <c r="G179" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.2">
@@ -3720,13 +3740,13 @@
         <v>186</v>
       </c>
       <c r="E180" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F180" t="s">
         <v>8</v>
       </c>
       <c r="G180" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.2">
@@ -3734,13 +3754,13 @@
         <v>187</v>
       </c>
       <c r="E181" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F181" t="s">
         <v>8</v>
       </c>
       <c r="G181" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="182" spans="3:7" x14ac:dyDescent="0.2">
@@ -3748,13 +3768,13 @@
         <v>188</v>
       </c>
       <c r="E182" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F182" t="s">
         <v>8</v>
       </c>
       <c r="G182" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="183" spans="3:7" x14ac:dyDescent="0.2">
@@ -3762,13 +3782,13 @@
         <v>189</v>
       </c>
       <c r="E183" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F183" t="s">
         <v>8</v>
       </c>
       <c r="G183" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="184" spans="3:7" x14ac:dyDescent="0.2">
@@ -3776,13 +3796,13 @@
         <v>190</v>
       </c>
       <c r="E184" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F184" t="s">
         <v>8</v>
       </c>
       <c r="G184" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="185" spans="3:7" x14ac:dyDescent="0.2">
@@ -3790,13 +3810,13 @@
         <v>191</v>
       </c>
       <c r="E185" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F185" t="s">
         <v>8</v>
       </c>
       <c r="G185" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.2">
@@ -3804,13 +3824,13 @@
         <v>192</v>
       </c>
       <c r="E186" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F186" t="s">
         <v>8</v>
       </c>
       <c r="G186" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.2">
@@ -3818,13 +3838,13 @@
         <v>193</v>
       </c>
       <c r="E187" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F187" t="s">
         <v>8</v>
       </c>
       <c r="G187" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.2">
@@ -3832,13 +3852,13 @@
         <v>194</v>
       </c>
       <c r="E188" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F188" t="s">
         <v>8</v>
       </c>
       <c r="G188" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.2">
@@ -3846,13 +3866,13 @@
         <v>195</v>
       </c>
       <c r="E189" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F189" t="s">
         <v>8</v>
       </c>
       <c r="G189" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="3:7" x14ac:dyDescent="0.2">
@@ -3860,13 +3880,13 @@
         <v>196</v>
       </c>
       <c r="E190" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F190" t="s">
         <v>8</v>
       </c>
       <c r="G190" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="191" spans="3:7" x14ac:dyDescent="0.2">
@@ -3874,13 +3894,13 @@
         <v>197</v>
       </c>
       <c r="E191" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F191" t="s">
         <v>8</v>
       </c>
       <c r="G191" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="192" spans="3:7" x14ac:dyDescent="0.2">
@@ -3888,13 +3908,13 @@
         <v>198</v>
       </c>
       <c r="E192" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F192" t="s">
         <v>8</v>
       </c>
       <c r="G192" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.2">
@@ -3902,13 +3922,13 @@
         <v>199</v>
       </c>
       <c r="E193" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F193" t="s">
         <v>8</v>
       </c>
       <c r="G193" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="194" spans="3:7" x14ac:dyDescent="0.2">
@@ -3916,13 +3936,13 @@
         <v>200</v>
       </c>
       <c r="E194" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F194" t="s">
         <v>8</v>
       </c>
       <c r="G194" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.2">
@@ -3930,13 +3950,13 @@
         <v>201</v>
       </c>
       <c r="E195" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F195" t="s">
         <v>8</v>
       </c>
       <c r="G195" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="196" spans="3:7" x14ac:dyDescent="0.2">
@@ -3944,13 +3964,13 @@
         <v>202</v>
       </c>
       <c r="E196" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F196" t="s">
         <v>8</v>
       </c>
       <c r="G196" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.2">
@@ -3958,13 +3978,13 @@
         <v>203</v>
       </c>
       <c r="E197" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F197" t="s">
         <v>8</v>
       </c>
       <c r="G197" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.2">
@@ -3972,13 +3992,13 @@
         <v>204</v>
       </c>
       <c r="E198" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F198" t="s">
         <v>8</v>
       </c>
       <c r="G198" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="199" spans="3:7" x14ac:dyDescent="0.2">
@@ -3986,13 +4006,13 @@
         <v>205</v>
       </c>
       <c r="E199" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F199" t="s">
         <v>8</v>
       </c>
       <c r="G199" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="200" spans="3:7" x14ac:dyDescent="0.2">
@@ -4000,13 +4020,13 @@
         <v>206</v>
       </c>
       <c r="E200" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="F200" t="s">
         <v>8</v>
       </c>
       <c r="G200" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="201" spans="3:7" x14ac:dyDescent="0.2">
@@ -4014,13 +4034,13 @@
         <v>207</v>
       </c>
       <c r="E201" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F201" t="s">
         <v>8</v>
       </c>
       <c r="G201" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="202" spans="3:7" x14ac:dyDescent="0.2">
@@ -4028,13 +4048,13 @@
         <v>209</v>
       </c>
       <c r="E202" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F202" t="s">
         <v>8</v>
       </c>
       <c r="G202" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="203" spans="3:7" x14ac:dyDescent="0.2">
@@ -4042,13 +4062,13 @@
         <v>210</v>
       </c>
       <c r="E203" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F203" t="s">
         <v>8</v>
       </c>
       <c r="G203" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="204" spans="3:7" x14ac:dyDescent="0.2">
@@ -4056,13 +4076,13 @@
         <v>211</v>
       </c>
       <c r="E204" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F204" t="s">
         <v>8</v>
       </c>
       <c r="G204" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="205" spans="3:7" x14ac:dyDescent="0.2">
@@ -4070,13 +4090,13 @@
         <v>212</v>
       </c>
       <c r="E205" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F205" t="s">
         <v>8</v>
       </c>
       <c r="G205" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="206" spans="3:7" x14ac:dyDescent="0.2">
@@ -4084,13 +4104,13 @@
         <v>213</v>
       </c>
       <c r="E206" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F206" t="s">
         <v>8</v>
       </c>
       <c r="G206" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="207" spans="3:7" x14ac:dyDescent="0.2">
@@ -4098,13 +4118,13 @@
         <v>214</v>
       </c>
       <c r="E207" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F207" t="s">
         <v>8</v>
       </c>
       <c r="G207" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="208" spans="3:7" x14ac:dyDescent="0.2">
@@ -4112,13 +4132,13 @@
         <v>215</v>
       </c>
       <c r="E208" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F208" t="s">
         <v>8</v>
       </c>
       <c r="G208" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="209" spans="3:7" x14ac:dyDescent="0.2">
@@ -4126,13 +4146,13 @@
         <v>216</v>
       </c>
       <c r="E209" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F209" t="s">
         <v>8</v>
       </c>
       <c r="G209" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="210" spans="3:7" x14ac:dyDescent="0.2">
@@ -4140,13 +4160,13 @@
         <v>217</v>
       </c>
       <c r="E210" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F210" t="s">
         <v>8</v>
       </c>
       <c r="G210" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="211" spans="3:7" x14ac:dyDescent="0.2">
@@ -4154,13 +4174,13 @@
         <v>218</v>
       </c>
       <c r="E211" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F211" t="s">
         <v>8</v>
       </c>
       <c r="G211" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="212" spans="3:7" x14ac:dyDescent="0.2">
@@ -4168,13 +4188,13 @@
         <v>219</v>
       </c>
       <c r="E212" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F212" t="s">
         <v>8</v>
       </c>
       <c r="G212" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="213" spans="3:7" x14ac:dyDescent="0.2">
@@ -4182,13 +4202,13 @@
         <v>220</v>
       </c>
       <c r="E213" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F213" t="s">
         <v>8</v>
       </c>
       <c r="G213" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="214" spans="3:7" x14ac:dyDescent="0.2">
@@ -4196,13 +4216,13 @@
         <v>221</v>
       </c>
       <c r="E214" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F214" t="s">
         <v>8</v>
       </c>
       <c r="G214" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="215" spans="3:7" x14ac:dyDescent="0.2">
@@ -4210,13 +4230,13 @@
         <v>222</v>
       </c>
       <c r="E215" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F215" t="s">
         <v>8</v>
       </c>
       <c r="G215" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="216" spans="3:7" x14ac:dyDescent="0.2">
@@ -4224,13 +4244,13 @@
         <v>223</v>
       </c>
       <c r="E216" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F216" t="s">
         <v>8</v>
       </c>
       <c r="G216" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="217" spans="3:7" x14ac:dyDescent="0.2">
@@ -4238,13 +4258,13 @@
         <v>224</v>
       </c>
       <c r="E217" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F217" t="s">
         <v>8</v>
       </c>
       <c r="G217" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="218" spans="3:7" x14ac:dyDescent="0.2">
@@ -4252,13 +4272,13 @@
         <v>225</v>
       </c>
       <c r="E218" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F218" t="s">
         <v>8</v>
       </c>
       <c r="G218" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="219" spans="3:7" x14ac:dyDescent="0.2">
@@ -4266,13 +4286,13 @@
         <v>226</v>
       </c>
       <c r="E219" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F219" t="s">
         <v>8</v>
       </c>
       <c r="G219" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="220" spans="3:7" x14ac:dyDescent="0.2">
@@ -4280,13 +4300,13 @@
         <v>227</v>
       </c>
       <c r="E220" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F220" t="s">
         <v>8</v>
       </c>
       <c r="G220" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="221" spans="3:7" x14ac:dyDescent="0.2">
@@ -4294,13 +4314,13 @@
         <v>228</v>
       </c>
       <c r="E221" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F221" t="s">
         <v>8</v>
       </c>
       <c r="G221" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="222" spans="3:7" x14ac:dyDescent="0.2">
@@ -4308,13 +4328,13 @@
         <v>229</v>
       </c>
       <c r="E222" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F222" t="s">
         <v>8</v>
       </c>
       <c r="G222" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="223" spans="3:7" x14ac:dyDescent="0.2">
@@ -4322,13 +4342,13 @@
         <v>230</v>
       </c>
       <c r="E223" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F223" t="s">
         <v>8</v>
       </c>
       <c r="G223" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="224" spans="3:7" x14ac:dyDescent="0.2">
@@ -4336,13 +4356,13 @@
         <v>231</v>
       </c>
       <c r="E224" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F224" t="s">
         <v>8</v>
       </c>
       <c r="G224" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="225" spans="3:7" x14ac:dyDescent="0.2">
@@ -4350,13 +4370,13 @@
         <v>232</v>
       </c>
       <c r="E225" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F225" t="s">
         <v>8</v>
       </c>
       <c r="G225" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="226" spans="3:7" x14ac:dyDescent="0.2">
@@ -4364,13 +4384,13 @@
         <v>233</v>
       </c>
       <c r="E226" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F226" t="s">
         <v>8</v>
       </c>
       <c r="G226" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="227" spans="3:7" x14ac:dyDescent="0.2">
@@ -4378,13 +4398,13 @@
         <v>234</v>
       </c>
       <c r="E227" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F227" t="s">
         <v>8</v>
       </c>
       <c r="G227" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="228" spans="3:7" x14ac:dyDescent="0.2">
@@ -4392,13 +4412,13 @@
         <v>235</v>
       </c>
       <c r="E228" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F228" t="s">
         <v>8</v>
       </c>
       <c r="G228" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="229" spans="3:7" x14ac:dyDescent="0.2">
@@ -4406,13 +4426,13 @@
         <v>236</v>
       </c>
       <c r="E229" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F229" t="s">
         <v>8</v>
       </c>
       <c r="G229" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="230" spans="3:7" x14ac:dyDescent="0.2">
@@ -4420,13 +4440,13 @@
         <v>237</v>
       </c>
       <c r="E230" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F230" t="s">
         <v>8</v>
       </c>
       <c r="G230" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="231" spans="3:7" x14ac:dyDescent="0.2">
@@ -4434,13 +4454,13 @@
         <v>238</v>
       </c>
       <c r="E231" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F231" t="s">
         <v>8</v>
       </c>
       <c r="G231" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="232" spans="3:7" x14ac:dyDescent="0.2">
@@ -4448,13 +4468,13 @@
         <v>239</v>
       </c>
       <c r="E232" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F232" t="s">
         <v>8</v>
       </c>
       <c r="G232" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="233" spans="3:7" x14ac:dyDescent="0.2">
@@ -4462,13 +4482,13 @@
         <v>240</v>
       </c>
       <c r="E233" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F233" t="s">
         <v>8</v>
       </c>
       <c r="G233" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="234" spans="3:7" x14ac:dyDescent="0.2">
@@ -4476,13 +4496,13 @@
         <v>241</v>
       </c>
       <c r="E234" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F234" t="s">
         <v>8</v>
       </c>
       <c r="G234" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="235" spans="3:7" x14ac:dyDescent="0.2">
@@ -4490,13 +4510,13 @@
         <v>242</v>
       </c>
       <c r="E235" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F235" t="s">
         <v>8</v>
       </c>
       <c r="G235" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="236" spans="3:7" x14ac:dyDescent="0.2">
@@ -4504,13 +4524,13 @@
         <v>243</v>
       </c>
       <c r="E236" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F236" t="s">
         <v>8</v>
       </c>
       <c r="G236" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="237" spans="3:7" x14ac:dyDescent="0.2">
@@ -4518,13 +4538,13 @@
         <v>244</v>
       </c>
       <c r="E237" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F237" t="s">
         <v>8</v>
       </c>
       <c r="G237" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="238" spans="3:7" x14ac:dyDescent="0.2">
@@ -4532,13 +4552,13 @@
         <v>245</v>
       </c>
       <c r="E238" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F238" t="s">
         <v>8</v>
       </c>
       <c r="G238" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="239" spans="3:7" x14ac:dyDescent="0.2">
@@ -4546,13 +4566,13 @@
         <v>246</v>
       </c>
       <c r="E239" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F239" t="s">
         <v>8</v>
       </c>
       <c r="G239" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="240" spans="3:7" x14ac:dyDescent="0.2">
@@ -4560,13 +4580,13 @@
         <v>247</v>
       </c>
       <c r="E240" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F240" t="s">
         <v>8</v>
       </c>
       <c r="G240" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="241" spans="3:7" x14ac:dyDescent="0.2">
@@ -4574,13 +4594,13 @@
         <v>248</v>
       </c>
       <c r="E241" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F241" t="s">
         <v>8</v>
       </c>
       <c r="G241" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="242" spans="3:7" x14ac:dyDescent="0.2">
@@ -4588,13 +4608,13 @@
         <v>249</v>
       </c>
       <c r="E242" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F242" t="s">
         <v>8</v>
       </c>
       <c r="G242" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="243" spans="3:7" x14ac:dyDescent="0.2">
@@ -4602,13 +4622,13 @@
         <v>250</v>
       </c>
       <c r="E243" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F243" t="s">
         <v>8</v>
       </c>
       <c r="G243" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="244" spans="3:7" x14ac:dyDescent="0.2">
@@ -4616,13 +4636,13 @@
         <v>251</v>
       </c>
       <c r="E244" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F244" t="s">
         <v>8</v>
       </c>
       <c r="G244" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="245" spans="3:7" x14ac:dyDescent="0.2">
@@ -4630,13 +4650,13 @@
         <v>252</v>
       </c>
       <c r="E245" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F245" t="s">
         <v>8</v>
       </c>
       <c r="G245" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="246" spans="3:7" x14ac:dyDescent="0.2">
@@ -4644,13 +4664,13 @@
         <v>253</v>
       </c>
       <c r="E246" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F246" t="s">
         <v>8</v>
       </c>
       <c r="G246" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="247" spans="3:7" x14ac:dyDescent="0.2">
@@ -4658,13 +4678,13 @@
         <v>254</v>
       </c>
       <c r="E247" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F247" t="s">
         <v>8</v>
       </c>
       <c r="G247" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="248" spans="3:7" x14ac:dyDescent="0.2">
@@ -4672,13 +4692,13 @@
         <v>255</v>
       </c>
       <c r="E248" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F248" t="s">
         <v>8</v>
       </c>
       <c r="G248" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="249" spans="3:7" x14ac:dyDescent="0.2">
@@ -4686,13 +4706,13 @@
         <v>256</v>
       </c>
       <c r="E249" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F249" t="s">
         <v>8</v>
       </c>
       <c r="G249" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="250" spans="3:7" x14ac:dyDescent="0.2">
@@ -4700,13 +4720,13 @@
         <v>257</v>
       </c>
       <c r="E250" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F250" t="s">
         <v>8</v>
       </c>
       <c r="G250" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="251" spans="3:7" x14ac:dyDescent="0.2">
@@ -4714,13 +4734,13 @@
         <v>258</v>
       </c>
       <c r="E251" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F251" t="s">
         <v>8</v>
       </c>
       <c r="G251" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="252" spans="3:7" x14ac:dyDescent="0.2">
@@ -4728,13 +4748,13 @@
         <v>259</v>
       </c>
       <c r="E252" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F252" t="s">
         <v>8</v>
       </c>
       <c r="G252" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="253" spans="3:7" x14ac:dyDescent="0.2">
@@ -4742,13 +4762,13 @@
         <v>260</v>
       </c>
       <c r="E253" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F253" t="s">
         <v>8</v>
       </c>
       <c r="G253" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="254" spans="3:7" x14ac:dyDescent="0.2">
@@ -4756,13 +4776,13 @@
         <v>261</v>
       </c>
       <c r="E254" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F254" t="s">
         <v>8</v>
       </c>
       <c r="G254" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="255" spans="3:7" x14ac:dyDescent="0.2">
@@ -4770,13 +4790,13 @@
         <v>262</v>
       </c>
       <c r="E255" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F255" t="s">
         <v>8</v>
       </c>
       <c r="G255" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="256" spans="3:7" x14ac:dyDescent="0.2">
@@ -4784,13 +4804,13 @@
         <v>263</v>
       </c>
       <c r="E256" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F256" t="s">
         <v>8</v>
       </c>
       <c r="G256" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="257" spans="3:7" x14ac:dyDescent="0.2">
@@ -4798,13 +4818,13 @@
         <v>264</v>
       </c>
       <c r="E257" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F257" t="s">
         <v>8</v>
       </c>
       <c r="G257" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="258" spans="3:7" x14ac:dyDescent="0.2">
@@ -4812,13 +4832,13 @@
         <v>265</v>
       </c>
       <c r="E258" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F258" t="s">
         <v>8</v>
       </c>
       <c r="G258" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="259" spans="3:7" x14ac:dyDescent="0.2">
@@ -4826,13 +4846,13 @@
         <v>266</v>
       </c>
       <c r="E259" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F259" t="s">
         <v>8</v>
       </c>
       <c r="G259" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="260" spans="3:7" x14ac:dyDescent="0.2">
@@ -4840,13 +4860,13 @@
         <v>267</v>
       </c>
       <c r="E260" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F260" t="s">
         <v>8</v>
       </c>
       <c r="G260" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="261" spans="3:7" x14ac:dyDescent="0.2">
@@ -4854,13 +4874,13 @@
         <v>268</v>
       </c>
       <c r="E261" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F261" t="s">
         <v>8</v>
       </c>
       <c r="G261" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="262" spans="3:7" x14ac:dyDescent="0.2">
@@ -4868,13 +4888,13 @@
         <v>269</v>
       </c>
       <c r="E262" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F262" t="s">
         <v>8</v>
       </c>
       <c r="G262" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="263" spans="3:7" x14ac:dyDescent="0.2">
@@ -4882,13 +4902,13 @@
         <v>270</v>
       </c>
       <c r="E263" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F263" t="s">
         <v>8</v>
       </c>
       <c r="G263" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="264" spans="3:7" x14ac:dyDescent="0.2">
@@ -4896,13 +4916,13 @@
         <v>271</v>
       </c>
       <c r="E264" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F264" t="s">
         <v>8</v>
       </c>
       <c r="G264" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="265" spans="3:7" x14ac:dyDescent="0.2">
@@ -4910,13 +4930,13 @@
         <v>272</v>
       </c>
       <c r="E265" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F265" t="s">
         <v>8</v>
       </c>
       <c r="G265" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="266" spans="3:7" x14ac:dyDescent="0.2">
@@ -4924,13 +4944,13 @@
         <v>273</v>
       </c>
       <c r="E266" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F266" t="s">
         <v>8</v>
       </c>
       <c r="G266" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="267" spans="3:7" x14ac:dyDescent="0.2">
@@ -4938,13 +4958,13 @@
         <v>274</v>
       </c>
       <c r="E267" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F267" t="s">
         <v>8</v>
       </c>
       <c r="G267" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="268" spans="3:7" x14ac:dyDescent="0.2">
@@ -4952,13 +4972,13 @@
         <v>275</v>
       </c>
       <c r="E268" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F268" t="s">
         <v>8</v>
       </c>
       <c r="G268" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="269" spans="3:7" x14ac:dyDescent="0.2">
@@ -4966,13 +4986,13 @@
         <v>276</v>
       </c>
       <c r="E269" t="s">
-        <v>208</v>
+        <v>279</v>
       </c>
       <c r="F269" t="s">
         <v>8</v>
       </c>
       <c r="G269" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for Shaconemo r256 update.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -52,55 +52,55 @@
     <t xml:space="preserve">Thomas Reerink</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: Age_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: Age_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">areacello</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: areacello</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: areacello</t>
   </si>
   <si>
     <t xml:space="preserve">basin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: basins</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: basins</t>
   </si>
   <si>
     <t xml:space="preserve">bigthetao</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: toce</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: toce</t>
   </si>
   <si>
     <t xml:space="preserve">bigthetaoga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sctemtot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sctemtot</t>
   </si>
   <si>
     <t xml:space="preserve">cfc11</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: CFC11_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: CFC11_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">cfc12</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: CFC12_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: CFC12_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">deptho</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: tpt_dep</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: tpt_dep</t>
   </si>
   <si>
     <t xml:space="preserve">diftrblo2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: aht2d_eiv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: aht2d_eiv</t>
   </si>
   <si>
     <t xml:space="preserve">diftrelo2d</t>
@@ -109,31 +109,31 @@
     <t xml:space="preserve">diftrxylo2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: aht2d</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: aht2d</t>
   </si>
   <si>
     <t xml:space="preserve">difvho</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: avt_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: avt_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvmo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: avm_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: avm_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvmto</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: av_wave_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: av_wave_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvso</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: avs_e3w</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: avs_e3w</t>
   </si>
   <si>
     <t xml:space="preserve">difvtrto</t>
@@ -142,139 +142,139 @@
     <t xml:space="preserve">dispkevfo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: dispkevfo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: dispkevfo</t>
   </si>
   <si>
     <t xml:space="preserve">dispkexyfo2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: dispkexyfo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: dispkexyfo</t>
   </si>
   <si>
     <t xml:space="preserve">evs</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: evap_ao_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: evap_ao_cea</t>
   </si>
   <si>
     <t xml:space="preserve">fgcfc11</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: qtr_CFC11</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: qtr_CFC11</t>
   </si>
   <si>
     <t xml:space="preserve">fgcfc12</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: qtr_CFC12</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: qtr_CFC12</t>
   </si>
   <si>
     <t xml:space="preserve">fgsf6</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: qtr_SF6</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: qtr_SF6</t>
   </si>
   <si>
     <t xml:space="preserve">ficeberg2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: iceberg_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: iceberg_cea</t>
   </si>
   <si>
     <t xml:space="preserve">flandice</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: iceshelf_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: iceshelf_cea</t>
   </si>
   <si>
     <t xml:space="preserve">friver</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: runoffs</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: runoffs</t>
   </si>
   <si>
     <t xml:space="preserve">fsitherm</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: fmmflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: fmmflx</t>
   </si>
   <si>
     <t xml:space="preserve">hcont300</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: hc300</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: hc300</t>
   </si>
   <si>
     <t xml:space="preserve">hfbasin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sopht_vt_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sopht_vt_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">hfbasinpmadv</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sophteiv_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sophteiv_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">hfds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: qt</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: qt</t>
   </si>
   <si>
     <t xml:space="preserve">hfevapds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: hflx_evap_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: hflx_evap_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfgeou</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: hfgeou</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: hfgeou</t>
   </si>
   <si>
     <t xml:space="preserve">hfibthermds2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: hflx_icb_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: hflx_icb_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfrainds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: hflx_rain_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: hflx_rain_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfrunoffds2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: hflx_rnf_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: hflx_rnf_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfsnthermds2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: hflx_snow_ao_cea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: hflx_snow_ao_cea</t>
   </si>
   <si>
     <t xml:space="preserve">hfx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: uadv_heattr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: uadv_heattr</t>
   </si>
   <si>
     <t xml:space="preserve">hfy</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: vadv_heattr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: vadv_heattr</t>
   </si>
   <si>
     <t xml:space="preserve">htovgyre</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sophtove_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sophtove_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">htovovrt</t>
@@ -283,37 +283,37 @@
     <t xml:space="preserve">masscello</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: masscello</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: masscello</t>
   </si>
   <si>
     <t xml:space="preserve">masso</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: scmastot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: scmastot</t>
   </si>
   <si>
     <t xml:space="preserve">mfo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: transport_masse_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: transport_masse_transect</t>
   </si>
   <si>
     <t xml:space="preserve">mlotst</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: mldr10_3</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: mldr10_3</t>
   </si>
   <si>
     <t xml:space="preserve">mlotstmax</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: mldr10_3max</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: mldr10_3max</t>
   </si>
   <si>
     <t xml:space="preserve">mlotstmin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: mldr10_3min</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: mldr10_3min</t>
   </si>
   <si>
     <t xml:space="preserve">mlotstsq</t>
@@ -322,139 +322,139 @@
     <t xml:space="preserve">msftbarot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: uoce_e3u_vsum_e2u_cumul</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: uoce_e3u_vsum_e2u_cumul</t>
   </si>
   <si>
     <t xml:space="preserve">msftyz</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: zomsf_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: zomsf_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">obvfsq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: bn2_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: bn2_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontempdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: ttrd_zdfp_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: ttrd_zdfp_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemppadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: ttrd_eivad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: ttrd_eivad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemppmdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: ttrd_iso_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: ttrd_iso_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemprmadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: ttrd_totad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: ttrd_totad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">ocontemptend</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: ttrd_tot_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: ttrd_tot_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">omldamax</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: mldkz5</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: mldkz5</t>
   </si>
   <si>
     <t xml:space="preserve">osaltdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: strd_zdfp_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: strd_zdfp_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osaltpadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: strd_eivad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: strd_eivad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osaltpmdiff</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: strd_iso_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: strd_iso_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osaltrmadvect</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: strd_totad_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: strd_totad_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">osalttend</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: strd_tot_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: strd_tot_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">pbo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: botpres</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: botpres</t>
   </si>
   <si>
     <t xml:space="preserve">rsdo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: qsr3d_e3t_SBC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: qsr3d_e3t_SBC</t>
   </si>
   <si>
     <t xml:space="preserve">rsntds</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: qsr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: qsr</t>
   </si>
   <si>
     <t xml:space="preserve">sf6</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: SF6_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: SF6_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">sfdsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: saltflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: saltflx</t>
   </si>
   <si>
     <t xml:space="preserve">sftof</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: iceconc_pct</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: iceconc_pct</t>
   </si>
   <si>
     <t xml:space="preserve">sltbasin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sopst_vs_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sopst_vs_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">sltnortha</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sopst_atl</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sopst_atl</t>
   </si>
   <si>
     <t xml:space="preserve">sltovgyre</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sopstove_3bsn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sopstove_3bsn</t>
   </si>
   <si>
     <t xml:space="preserve">sltovovrt</t>
@@ -463,211 +463,211 @@
     <t xml:space="preserve">so</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: soce_e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: soce_e3t</t>
   </si>
   <si>
     <t xml:space="preserve">sob</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sbs_e3tb</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sbs_e3tb</t>
   </si>
   <si>
     <t xml:space="preserve">soga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: scsaltot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: scsaltot</t>
   </si>
   <si>
     <t xml:space="preserve">somint</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: somint</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: somint</t>
   </si>
   <si>
     <t xml:space="preserve">sos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sss</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sss</t>
   </si>
   <si>
     <t xml:space="preserve">sosga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: scssstot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: scssstot</t>
   </si>
   <si>
     <t xml:space="preserve">sossq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sss2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sss2</t>
   </si>
   <si>
     <t xml:space="preserve">t20d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: 20d</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: 20d</t>
   </si>
   <si>
     <t xml:space="preserve">tauuo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: utau</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: utau</t>
   </si>
   <si>
     <t xml:space="preserve">tauvo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: vtau</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: vtau</t>
   </si>
   <si>
     <t xml:space="preserve">thetao</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: toce_pot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: toce_pot</t>
   </si>
   <si>
     <t xml:space="preserve">thetaoga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sctemtotpot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sctemtotpot</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: toce_pot_vmean</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: toce_pot_vmean</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot2000</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: toce_pot_vmean2000</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: toce_pot_vmean2000</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot300</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: toce_pot_vmean300</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: toce_pot_vmean300</t>
   </si>
   <si>
     <t xml:space="preserve">thetaot700</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: toce_pot_vmean700</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: toce_pot_vmean700</t>
   </si>
   <si>
     <t xml:space="preserve">thkcello</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: e3t</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: e3t</t>
   </si>
   <si>
     <t xml:space="preserve">tnkebto2d</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: eketrd_eiv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: eketrd_eiv</t>
   </si>
   <si>
     <t xml:space="preserve">tnpeo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: tnpeo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: tnpeo</t>
   </si>
   <si>
     <t xml:space="preserve">tob</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: toce_potb_e3tb</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: toce_potb_e3tb</t>
   </si>
   <si>
     <t xml:space="preserve">tomint</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: tosmint</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: tosmint</t>
   </si>
   <si>
     <t xml:space="preserve">tos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sst_pot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sst_pot</t>
   </si>
   <si>
     <t xml:space="preserve">tosga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: scssttot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: scssttot</t>
   </si>
   <si>
     <t xml:space="preserve">tossq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sst_pot2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sst_pot2</t>
   </si>
   <si>
     <t xml:space="preserve">umo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: uocetr_eff</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: uocetr_eff</t>
   </si>
   <si>
     <t xml:space="preserve">uo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: uoce_e3u</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: uoce_e3u</t>
   </si>
   <si>
     <t xml:space="preserve">vmo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: vocetr_eff</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: vocetr_eff</t>
   </si>
   <si>
     <t xml:space="preserve">vo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: voce_e3v</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: voce_e3v</t>
   </si>
   <si>
     <t xml:space="preserve">volo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: scvoltot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: scvoltot</t>
   </si>
   <si>
     <t xml:space="preserve">wfonocorr</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: empmr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: empmr</t>
   </si>
   <si>
     <t xml:space="preserve">wmo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: wocetr_eff</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: wocetr_eff</t>
   </si>
   <si>
     <t xml:space="preserve">wo</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: woce</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: woce</t>
   </si>
   <si>
     <t xml:space="preserve">zos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sshdyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sshdyn</t>
   </si>
   <si>
     <t xml:space="preserve">zossq</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: sshdyn2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: sshdyn2</t>
   </si>
   <si>
     <t xml:space="preserve">zostoga</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocean ping file: scsshtst</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocean ping file: scsshtst</t>
   </si>
   <si>
     <t xml:space="preserve">bfe</t>
@@ -676,49 +676,49 @@
     <t xml:space="preserve">ocnBgChem</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: BFe_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: BFe_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: BFeSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: BFeSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: GSi_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: GSi_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bsios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: GSiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: GSiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">calc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: CaCO3_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: CaCO3_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chl</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NCHL_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NCHL_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chldiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: DCHL_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DCHL_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chldiatos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: DCHLSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DCHLSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chlmisc</t>
@@ -727,7 +727,7 @@
     <t xml:space="preserve">chlmiscos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NCHLSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NCHLSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chlos</t>
@@ -736,325 +736,325 @@
     <t xml:space="preserve">co3</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: CO3</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: CO3</t>
   </si>
   <si>
     <t xml:space="preserve">co3satcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: CO3sat</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: CO3sat</t>
   </si>
   <si>
     <t xml:space="preserve">dcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PCAL</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PCAL</t>
   </si>
   <si>
     <t xml:space="preserve">detoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: POC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: POC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: Fer_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Fer_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: FerSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: FerSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: DIC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DIC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissicos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: DICSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DICSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: DOC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DOC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dpco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: Dpco2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Dpco2</t>
   </si>
   <si>
     <t xml:space="preserve">dpo2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: Dpo2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Dpo2</t>
   </si>
   <si>
     <t xml:space="preserve">epc100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EPC100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPC100</t>
   </si>
   <si>
     <t xml:space="preserve">epcalc100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EPCAL100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPCAL100</t>
   </si>
   <si>
     <t xml:space="preserve">epfe100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EPFE100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPFE100</t>
   </si>
   <si>
     <t xml:space="preserve">epsi100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EPSI100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPSI100</t>
   </si>
   <si>
     <t xml:space="preserve">expc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EXPC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPC</t>
   </si>
   <si>
     <t xml:space="preserve">expcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EXPCAL</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPCAL</t>
   </si>
   <si>
     <t xml:space="preserve">expfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EXPFE</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPFE</t>
   </si>
   <si>
     <t xml:space="preserve">expsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: EXPSI</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPSI</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtalk</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTdtAlk</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtAlk</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTdtDIC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtDIC</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdife</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTdtFer</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtFer</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTdtDIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtDIN</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdip</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTdtDIP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtDIP</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdisi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTdtSil</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtSil</t>
   </si>
   <si>
     <t xml:space="preserve">fgco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: Cflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Cflx</t>
   </si>
   <si>
     <t xml:space="preserve">fgo2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: Oflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Oflx</t>
   </si>
   <si>
     <t xml:space="preserve">fric</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: SedCal</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: SedCal</t>
   </si>
   <si>
     <t xml:space="preserve">froc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: SedC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: SedC</t>
   </si>
   <si>
     <t xml:space="preserve">fsfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: IronSupply</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: IronSupply</t>
   </si>
   <si>
     <t xml:space="preserve">fsn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NitrSupply</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NitrSupply</t>
   </si>
   <si>
     <t xml:space="preserve">graz</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: GRAZ1</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: GRAZ1</t>
   </si>
   <si>
     <t xml:space="preserve">intdic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTDIC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTDIC</t>
   </si>
   <si>
     <t xml:space="preserve">intpbfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTPBFE</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPBFE</t>
   </si>
   <si>
     <t xml:space="preserve">intpbsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTPBSI</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPBSI</t>
   </si>
   <si>
     <t xml:space="preserve">intpn2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTNFIX</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTNFIX</t>
   </si>
   <si>
     <t xml:space="preserve">intpp</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTPP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPP</t>
   </si>
   <si>
     <t xml:space="preserve">intppdiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTPPPHY2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPPPHY2</t>
   </si>
   <si>
     <t xml:space="preserve">intppmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTPPPHY</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">intppnitrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: INTPNEW</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPNEW</t>
   </si>
   <si>
     <t xml:space="preserve">limfediat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: LDFeSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LDFeSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limfemisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: LNFeSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LNFeSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limirrdiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: LDlightSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LDlightSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limirrmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: LNlightSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LNlightSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limndiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: LDnutSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LDnutSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limnmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: LNnutSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LNnutSFC</t>
   </si>
   <si>
     <t xml:space="preserve">nh4</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NH4_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NH4_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">no3</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NO3_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NO3_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">no3os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NO3SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NO3SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">o2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: O2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: O2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">o2min</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: O2MIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: O2MIN</t>
   </si>
   <si>
     <t xml:space="preserve">o2os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: O2SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: O2SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pbfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PFeN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PFeN</t>
   </si>
   <si>
     <t xml:space="preserve">pbsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PBSi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PBSi</t>
   </si>
   <si>
     <t xml:space="preserve">pcalc</t>
@@ -1063,43 +1063,43 @@
     <t xml:space="preserve">pdi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PPPHY2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PPPHY2</t>
   </si>
   <si>
     <t xml:space="preserve">ph</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PH</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PH</t>
   </si>
   <si>
     <t xml:space="preserve">phyc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PHY_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PHY_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phycos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PHYSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PHYSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phydiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PHY2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PHY2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phyfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NFe_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NFe_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phyfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: NFeSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NFeSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phymisc</t>
@@ -1108,25 +1108,25 @@
     <t xml:space="preserve">physi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: DSi_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DSi_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">physios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: DSiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DSiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pnitrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: TPNEW</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: TPNEW</t>
   </si>
   <si>
     <t xml:space="preserve">po4</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PO4_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PO4_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">poc</t>
@@ -1135,13 +1135,13 @@
     <t xml:space="preserve">pocos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: POCSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: POCSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pp</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: TPP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: TPP</t>
   </si>
   <si>
     <t xml:space="preserve">ppdiat</t>
@@ -1150,55 +1150,55 @@
     <t xml:space="preserve">ppmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: PPPHY</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">remoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: REMIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: REMIN</t>
   </si>
   <si>
     <t xml:space="preserve">si</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: Si_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Si_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">sios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: SiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: SiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">spco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: pCO2sea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: pCO2sea</t>
   </si>
   <si>
     <t xml:space="preserve">talk</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: Alkalini_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Alkalini_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmeso</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: ZOO2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: ZOO2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmicro</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: ZOO_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: ZOO_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zo2min</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) ocnBgChem ping file: ZO2MIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: ZO2MIN</t>
   </si>
   <si>
     <t xml:space="preserve">zooc</t>
@@ -1210,415 +1210,415 @@
     <t xml:space="preserve">seaIce</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: iceage</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: iceage</t>
   </si>
   <si>
     <t xml:space="preserve">siareaacrossline</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: transport_siarea_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: transport_siarea_transect</t>
   </si>
   <si>
     <t xml:space="preserve">siarean</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: NH_icearea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: NH_sc_icearea</t>
   </si>
   <si>
     <t xml:space="preserve">siareas</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: SH_icearea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: SH_sc_icearea</t>
   </si>
   <si>
     <t xml:space="preserve">sicompstren</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icestr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icestr</t>
   </si>
   <si>
     <t xml:space="preserve">siconc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: iceconc_pct</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: iceconc_pct</t>
   </si>
   <si>
     <t xml:space="preserve">sidconcdyn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: afxdyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: afxdyn</t>
   </si>
   <si>
     <t xml:space="preserve">sidconcth</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: afxthd</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: afxthd</t>
   </si>
   <si>
     <t xml:space="preserve">sidivvel</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: idive</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: idive</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassdyn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmidyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmidyn</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassevapsubl</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmisub</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmisub</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassgrowthbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmibog</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmibog</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassgrowthwat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmiopw</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmiopw</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassmeltbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmibom</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmibom</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassmelttop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmisum</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmisum</t>
   </si>
   <si>
     <t xml:space="preserve">sidmasssi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmisni</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmisni</t>
   </si>
   <si>
     <t xml:space="preserve">sidmassth</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmithd</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmithd</t>
   </si>
   <si>
     <t xml:space="preserve">sidmasstranx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: xmtrptot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: xmtrptot</t>
   </si>
   <si>
     <t xml:space="preserve">sidmasstrany</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: ymtrptot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: ymtrptot</t>
   </si>
   <si>
     <t xml:space="preserve">siextentn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: NH_iceextt</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: NH_sc_iceextt</t>
   </si>
   <si>
     <t xml:space="preserve">siextents</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: SH_iceextt</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: SH_sc_iceextt</t>
   </si>
   <si>
     <t xml:space="preserve">sifb</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icefb</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icefb</t>
   </si>
   <si>
     <t xml:space="preserve">siflcondbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: hfxconbo</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: hfxconbo</t>
   </si>
   <si>
     <t xml:space="preserve">siflcondtop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: hfxconsu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: hfxconsu</t>
   </si>
   <si>
     <t xml:space="preserve">siflfwbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: wfxtot</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: wfxtot</t>
   </si>
   <si>
     <t xml:space="preserve">siflfwdrain</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: wfxsum</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: wfxsum</t>
   </si>
   <si>
     <t xml:space="preserve">siflsaltbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: sfx_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: sfx_mv</t>
   </si>
   <si>
     <t xml:space="preserve">siflsensupbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: hfxsenso</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: hfxsenso</t>
   </si>
   <si>
     <t xml:space="preserve">siforcecoriolx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: corstrx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: corstrx</t>
   </si>
   <si>
     <t xml:space="preserve">siforcecorioly</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: corstry</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: corstry</t>
   </si>
   <si>
     <t xml:space="preserve">siforceintstrx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: intstrx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: intstrx</t>
   </si>
   <si>
     <t xml:space="preserve">siforceintstry</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: intstry</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: intstry</t>
   </si>
   <si>
     <t xml:space="preserve">siforcetiltx</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dssh_dx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dssh_dx</t>
   </si>
   <si>
     <t xml:space="preserve">siforcetilty</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dssh_dy</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dssh_dy</t>
   </si>
   <si>
     <t xml:space="preserve">sihc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icehcneg</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icehcneg</t>
   </si>
   <si>
     <t xml:space="preserve">siitdconc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: iceconc_cat_pct_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: iceconc_cat_pct_mv</t>
   </si>
   <si>
     <t xml:space="preserve">siitdsnthick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: snowthic_cat_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: snowthic_cat_mv</t>
   </si>
   <si>
     <t xml:space="preserve">siitdthick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icethic_cat_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icethic_cat_mv</t>
   </si>
   <si>
     <t xml:space="preserve">simass</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icemass</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icemass</t>
   </si>
   <si>
     <t xml:space="preserve">simassacrossline</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: transport_simasse_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: transport_simasse_transect</t>
   </si>
   <si>
     <t xml:space="preserve">sisali</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icesal</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icesal</t>
   </si>
   <si>
     <t xml:space="preserve">sisaltmass</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icesmass</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icesmass</t>
   </si>
   <si>
     <t xml:space="preserve">sishevel</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: ishear</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: ishear</t>
   </si>
   <si>
     <t xml:space="preserve">sisnhc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: isnhcneg</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: isnhcneg</t>
   </si>
   <si>
     <t xml:space="preserve">sisnmass</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: snomass</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: snomass</t>
   </si>
   <si>
     <t xml:space="preserve">sisnthick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: snothic</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: snothic</t>
   </si>
   <si>
     <t xml:space="preserve">sispeed</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icevel_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icevel_mv</t>
   </si>
   <si>
     <t xml:space="preserve">sistremax</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: sheastr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: sheastr</t>
   </si>
   <si>
     <t xml:space="preserve">sistresave</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: normstr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: normstr</t>
   </si>
   <si>
     <t xml:space="preserve">sistrxdtop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: utau_ice</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: utau_ice</t>
   </si>
   <si>
     <t xml:space="preserve">sistrxubot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: utau_oi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: utau_oi</t>
   </si>
   <si>
     <t xml:space="preserve">sistrydtop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: vtau_ice</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: vtau_ice</t>
   </si>
   <si>
     <t xml:space="preserve">sistryubot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: vtau_oi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: vtau_oi</t>
   </si>
   <si>
     <t xml:space="preserve">sitempbot</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icebotK</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icebotK</t>
   </si>
   <si>
     <t xml:space="preserve">sitempsnic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icesntK</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icesntK</t>
   </si>
   <si>
     <t xml:space="preserve">sitemptop</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icestK</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icestK</t>
   </si>
   <si>
     <t xml:space="preserve">sithick</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icethic</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icethic</t>
   </si>
   <si>
     <t xml:space="preserve">sitimefrac</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icepres</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icepres</t>
   </si>
   <si>
     <t xml:space="preserve">siu</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: uice_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: uice_mv</t>
   </si>
   <si>
     <t xml:space="preserve">siv</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: vice_mv</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: vice_mv</t>
   </si>
   <si>
     <t xml:space="preserve">sivol</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: icevolu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: icevolu</t>
   </si>
   <si>
     <t xml:space="preserve">sivoln</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: NH_icevolu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: NH_sc_icevolu</t>
   </si>
   <si>
     <t xml:space="preserve">sivols</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: SH_icevolu</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: SH_sc_icevolu</t>
   </si>
   <si>
     <t xml:space="preserve">sndmassdyn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmsdyn</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmsdyn</t>
   </si>
   <si>
     <t xml:space="preserve">sndmassmelt</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmsmel</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmsmel</t>
   </si>
   <si>
     <t xml:space="preserve">sndmasssi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmsssi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmsssi</t>
   </si>
   <si>
     <t xml:space="preserve">sndmasssnf</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmsspr</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmsspr</t>
   </si>
   <si>
     <t xml:space="preserve">sndmasssubl</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: dmssub</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: dmssub</t>
   </si>
   <si>
     <t xml:space="preserve">snmassacrossline</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r255) seaIce ping file: transport_snmasse_transect</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) seaIce ping file: transport_snmasse_transect</t>
   </si>
 </sst>
 </file>
@@ -1730,13 +1730,13 @@
   </sheetPr>
   <dimension ref="A1:G269"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.66"/>

</xml_diff>

<commit_message>
Change due to the awkward data request update: ocnBgChem => ocnBgchem #187
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -673,52 +673,52 @@
     <t xml:space="preserve">bfe</t>
   </si>
   <si>
-    <t xml:space="preserve">ocnBgChem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: BFe_E3T</t>
+    <t xml:space="preserve">ocnBgchem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: BFe_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: BFeSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: BFeSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: GSi_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: GSi_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">bsios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: GSiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: GSiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">calc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: CaCO3_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: CaCO3_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chl</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NCHL_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NCHL_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chldiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DCHL_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: DCHL_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chldiatos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DCHLSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: DCHLSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chlmisc</t>
@@ -727,7 +727,7 @@
     <t xml:space="preserve">chlmiscos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NCHLSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NCHLSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">chlos</t>
@@ -736,325 +736,325 @@
     <t xml:space="preserve">co3</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: CO3</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: CO3</t>
   </si>
   <si>
     <t xml:space="preserve">co3satcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: CO3sat</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: CO3sat</t>
   </si>
   <si>
     <t xml:space="preserve">dcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PCAL</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PCAL</t>
   </si>
   <si>
     <t xml:space="preserve">detoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: POC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: POC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Fer_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: Fer_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: FerSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: FerSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DIC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: DIC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissicos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DICSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: DICSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DOC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: DOC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dpco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Dpco2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: Dpco2</t>
   </si>
   <si>
     <t xml:space="preserve">dpo2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Dpo2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: Dpo2</t>
   </si>
   <si>
     <t xml:space="preserve">epc100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPC100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EPC100</t>
   </si>
   <si>
     <t xml:space="preserve">epcalc100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPCAL100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EPCAL100</t>
   </si>
   <si>
     <t xml:space="preserve">epfe100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPFE100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EPFE100</t>
   </si>
   <si>
     <t xml:space="preserve">epsi100</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EPSI100</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EPSI100</t>
   </si>
   <si>
     <t xml:space="preserve">expc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EXPC</t>
   </si>
   <si>
     <t xml:space="preserve">expcalc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPCAL</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EXPCAL</t>
   </si>
   <si>
     <t xml:space="preserve">expfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPFE</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EXPFE</t>
   </si>
   <si>
     <t xml:space="preserve">expsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: EXPSI</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: EXPSI</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtalk</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtAlk</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTdtAlk</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtDIC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTdtDIC</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdife</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtFer</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTdtFer</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdin</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtDIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTdtDIN</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdip</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtDIP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTdtDIP</t>
   </si>
   <si>
     <t xml:space="preserve">fbddtdisi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTdtSil</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTdtSil</t>
   </si>
   <si>
     <t xml:space="preserve">fgco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Cflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: Cflx</t>
   </si>
   <si>
     <t xml:space="preserve">fgo2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Oflx</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: Oflx</t>
   </si>
   <si>
     <t xml:space="preserve">fric</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: SedCal</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: SedCal</t>
   </si>
   <si>
     <t xml:space="preserve">froc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: SedC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: SedC</t>
   </si>
   <si>
     <t xml:space="preserve">fsfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: IronSupply</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: IronSupply</t>
   </si>
   <si>
     <t xml:space="preserve">fsn</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NitrSupply</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NitrSupply</t>
   </si>
   <si>
     <t xml:space="preserve">graz</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: GRAZ1</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: GRAZ1</t>
   </si>
   <si>
     <t xml:space="preserve">intdic</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTDIC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTDIC</t>
   </si>
   <si>
     <t xml:space="preserve">intpbfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPBFE</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTPBFE</t>
   </si>
   <si>
     <t xml:space="preserve">intpbsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPBSI</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTPBSI</t>
   </si>
   <si>
     <t xml:space="preserve">intpn2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTNFIX</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTNFIX</t>
   </si>
   <si>
     <t xml:space="preserve">intpp</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTPP</t>
   </si>
   <si>
     <t xml:space="preserve">intppdiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPPPHY2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTPPPHY2</t>
   </si>
   <si>
     <t xml:space="preserve">intppmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPPPHY</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTPPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">intppnitrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: INTPNEW</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: INTPNEW</t>
   </si>
   <si>
     <t xml:space="preserve">limfediat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LDFeSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: LDFeSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limfemisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LNFeSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: LNFeSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limirrdiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LDlightSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: LDlightSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limirrmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LNlightSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: LNlightSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limndiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LDnutSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: LDnutSFC</t>
   </si>
   <si>
     <t xml:space="preserve">limnmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: LNnutSFC</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: LNnutSFC</t>
   </si>
   <si>
     <t xml:space="preserve">nh4</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NH4_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NH4_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">no3</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NO3_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NO3_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">no3os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NO3SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NO3SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">o2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: O2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: O2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">o2min</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: O2MIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: O2MIN</t>
   </si>
   <si>
     <t xml:space="preserve">o2os</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: O2SFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: O2SFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pbfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PFeN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PFeN</t>
   </si>
   <si>
     <t xml:space="preserve">pbsi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PBSi</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PBSi</t>
   </si>
   <si>
     <t xml:space="preserve">pcalc</t>
@@ -1063,43 +1063,43 @@
     <t xml:space="preserve">pdi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PPPHY2</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PPPHY2</t>
   </si>
   <si>
     <t xml:space="preserve">ph</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PH</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PH</t>
   </si>
   <si>
     <t xml:space="preserve">phyc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PHY_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PHY_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phycos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PHYSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PHYSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phydiat</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PHY2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PHY2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phyfe</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NFe_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NFe_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phyfeos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: NFeSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: NFeSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">phymisc</t>
@@ -1108,25 +1108,25 @@
     <t xml:space="preserve">physi</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DSi_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: DSi_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">physios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: DSiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: DSiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pnitrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: TPNEW</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: TPNEW</t>
   </si>
   <si>
     <t xml:space="preserve">po4</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PO4_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PO4_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">poc</t>
@@ -1135,13 +1135,13 @@
     <t xml:space="preserve">pocos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: POCSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: POCSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">pp</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: TPP</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: TPP</t>
   </si>
   <si>
     <t xml:space="preserve">ppdiat</t>
@@ -1150,55 +1150,55 @@
     <t xml:space="preserve">ppmisc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: PPPHY</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: PPPHY</t>
   </si>
   <si>
     <t xml:space="preserve">remoc</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: REMIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: REMIN</t>
   </si>
   <si>
     <t xml:space="preserve">si</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Si_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: Si_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">sios</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: SiSFC_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: SiSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">spco2</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: pCO2sea</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: pCO2sea</t>
   </si>
   <si>
     <t xml:space="preserve">talk</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: Alkalini_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: Alkalini_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmeso</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: ZOO2_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: ZOO2_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmicro</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: ZOO_E3T</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: ZOO_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zo2min</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgChem ping file: ZO2MIN</t>
+    <t xml:space="preserve">Identified in the shaconemo (r256) ocnBgchem ping file: ZO2MIN</t>
   </si>
   <si>
     <t xml:space="preserve">zooc</t>
@@ -1702,13 +1702,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1730,20 +1734,20 @@
   </sheetPr>
   <dimension ref="A1:G269"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C269"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E120" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E109" activeCellId="0" sqref="E109:E200 G109:G200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="80.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="80.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.165991902834"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="81.4089068825911"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="81.4089068825911"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.67611336032389"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,7 +3261,7 @@
       <c r="C109" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="E109" s="0" t="s">
+      <c r="E109" s="2" t="s">
         <v>217</v>
       </c>
       <c r="F109" s="0" t="s">
@@ -5510,7 +5514,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Remove a doubling of snmassacrossline in the nemo-only-pre-list-of-identified-missing list.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="894">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -2816,10 +2816,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N297"/>
+  <dimension ref="A1:N296"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A297" activeCellId="0" sqref="297:297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8780,26 +8780,6 @@
         <v>893</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B297" s="0" t="s">
-        <v>891</v>
-      </c>
-      <c r="H297" s="0" t="s">
-        <v>892</v>
-      </c>
-      <c r="I297" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L297" s="0" t="s">
-        <v>681</v>
-      </c>
-      <c r="M297" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="N297" s="0" t="s">
-        <v>893</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Full reprocessed nemo-only-pre-list-of-identified-missing list from current ec-earth ping files, including the add of the now non-dummy dissicnat & talknat #521.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-only-pre-list-of-identified-missing-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="894">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -1309,21 +1309,21 @@
     <t xml:space="preserve"> P1 (mol m-3) mole_concentration_of_dissolved_inorganic_carbon_in_sea_water : Dissolved inorganic carbon (CO3+HCO3+H2CO3) concentration </t>
   </si>
   <si>
+    <t xml:space="preserve">dissicnat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P1 (mol m-3) mole_concentration_of_dissolved_inorganic_carbon_natural_analogue_in_sea_water : Dissolved inorganic carbon (CO3+HCO3+H2CO3) concentration at preindustrial atmospheric xCO2 </t>
+  </si>
+  <si>
     <t xml:space="preserve">dissicnatos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> P1 (mol m-3) mole_concentration_of_dissolved_inorganic_carbon_natural_analogue_in_sea_water : Dissolved inorganic carbon (CO3+HCO3+H2CO3) concentration at preindustrial atmospheric xCO2 </t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DICSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">dissicos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: DICSFC_E3T</t>
-  </si>
-  <si>
     <t xml:space="preserve">dissoc</t>
   </si>
   <si>
@@ -1987,19 +1987,19 @@
     <t xml:space="preserve"> P1 (mol m-3) sea_water_alkalinity_expressed_as_mole_equivalent : total alkalinity equivalent concentration (including carbonate, borate, phosphorus, silicon, and nitrogen components) </t>
   </si>
   <si>
+    <t xml:space="preserve">talknat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P1 (mol m-3) sea_water_alkalinity_natural_analogue_expressed_as_mole_equivalent : total alkalinity equivalent concentration (including carbonate, borate, phosphorus, silicon, and nitrogen components) at preindustrial atmospheric xCO2 </t>
+  </si>
+  <si>
     <t xml:space="preserve">talknatos</t>
   </si>
   <si>
-    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: Alkalini</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> P1 (mol m-3) sea_water_alkalinity_natural_analogue_expressed_as_mole_equivalent : total alkalinity equivalent concentration (including carbonate, borate, phosphorus, silicon, and nitrogen components) at preindustrial atmospheric xCO2 </t>
+    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: AlkaliniSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">talkos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identified in the shaconemo (r274) ocnBgchem ping file: AlkaliniSFC_E3T</t>
   </si>
   <si>
     <t xml:space="preserve">zmeso</t>
@@ -2816,10 +2816,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N296"/>
+  <dimension ref="A1:N298"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A297" activeCellId="0" sqref="297:297"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M275" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M298" activeCellId="0" sqref="298:298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5605,7 +5605,7 @@
         <v>429</v>
       </c>
       <c r="H138" s="0" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="I138" s="0" t="s">
         <v>16</v>
@@ -5617,15 +5617,15 @@
         <v>35</v>
       </c>
       <c r="N138" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="H139" s="0" t="s">
         <v>432</v>
-      </c>
-      <c r="H139" s="0" t="s">
-        <v>433</v>
       </c>
       <c r="I139" s="0" t="s">
         <v>16</v>
@@ -5637,15 +5637,15 @@
         <v>35</v>
       </c>
       <c r="N139" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H140" s="0" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I140" s="0" t="s">
         <v>16</v>
@@ -5657,15 +5657,15 @@
         <v>35</v>
       </c>
       <c r="N140" s="0" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="0" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H141" s="0" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I141" s="0" t="s">
         <v>16</v>
@@ -5677,15 +5677,15 @@
         <v>35</v>
       </c>
       <c r="N141" s="0" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="0" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="H142" s="0" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I142" s="0" t="s">
         <v>16</v>
@@ -5694,18 +5694,18 @@
         <v>369</v>
       </c>
       <c r="M142" s="0" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="N142" s="0" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="0" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="H143" s="0" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="I143" s="0" t="s">
         <v>16</v>
@@ -5717,15 +5717,15 @@
         <v>219</v>
       </c>
       <c r="N143" s="0" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="0" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H144" s="0" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="I144" s="0" t="s">
         <v>16</v>
@@ -5734,18 +5734,18 @@
         <v>369</v>
       </c>
       <c r="M144" s="0" t="s">
-        <v>448</v>
+        <v>219</v>
       </c>
       <c r="N144" s="0" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H145" s="0" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="I145" s="0" t="s">
         <v>16</v>
@@ -5757,15 +5757,15 @@
         <v>448</v>
       </c>
       <c r="N145" s="0" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="0" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H146" s="0" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I146" s="0" t="s">
         <v>16</v>
@@ -5777,15 +5777,15 @@
         <v>448</v>
       </c>
       <c r="N146" s="0" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="0" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H147" s="0" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I147" s="0" t="s">
         <v>16</v>
@@ -5797,15 +5797,15 @@
         <v>448</v>
       </c>
       <c r="N147" s="0" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="0" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H148" s="0" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I148" s="0" t="s">
         <v>16</v>
@@ -5817,15 +5817,15 @@
         <v>448</v>
       </c>
       <c r="N148" s="0" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="0" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H149" s="0" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="I149" s="0" t="s">
         <v>16</v>
@@ -5837,15 +5837,15 @@
         <v>448</v>
       </c>
       <c r="N149" s="0" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="0" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="H150" s="0" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I150" s="0" t="s">
         <v>16</v>
@@ -5857,15 +5857,15 @@
         <v>448</v>
       </c>
       <c r="N150" s="0" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="0" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H151" s="0" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="I151" s="0" t="s">
         <v>16</v>
@@ -5877,12 +5877,12 @@
         <v>448</v>
       </c>
       <c r="N151" s="0" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="0" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H152" s="0" t="s">
         <v>460</v>
@@ -5897,15 +5897,15 @@
         <v>448</v>
       </c>
       <c r="N152" s="0" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="0" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H153" s="0" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="I153" s="0" t="s">
         <v>16</v>
@@ -5917,15 +5917,15 @@
         <v>448</v>
       </c>
       <c r="N153" s="0" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="0" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H154" s="0" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I154" s="0" t="s">
         <v>16</v>
@@ -5937,15 +5937,15 @@
         <v>448</v>
       </c>
       <c r="N154" s="0" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="0" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H155" s="0" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I155" s="0" t="s">
         <v>16</v>
@@ -5957,15 +5957,15 @@
         <v>448</v>
       </c>
       <c r="N155" s="0" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="0" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H156" s="0" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I156" s="0" t="s">
         <v>16</v>
@@ -5977,15 +5977,15 @@
         <v>448</v>
       </c>
       <c r="N156" s="0" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="0" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H157" s="0" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I157" s="0" t="s">
         <v>16</v>
@@ -5997,15 +5997,15 @@
         <v>448</v>
       </c>
       <c r="N157" s="0" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="0" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H158" s="0" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I158" s="0" t="s">
         <v>16</v>
@@ -6017,15 +6017,15 @@
         <v>448</v>
       </c>
       <c r="N158" s="0" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="0" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H159" s="0" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I159" s="0" t="s">
         <v>16</v>
@@ -6037,15 +6037,15 @@
         <v>448</v>
       </c>
       <c r="N159" s="0" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="0" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="H160" s="0" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I160" s="0" t="s">
         <v>16</v>
@@ -6054,18 +6054,18 @@
         <v>369</v>
       </c>
       <c r="M160" s="0" t="s">
-        <v>76</v>
+        <v>448</v>
       </c>
       <c r="N160" s="0" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="0" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H161" s="0" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I161" s="0" t="s">
         <v>16</v>
@@ -6074,18 +6074,18 @@
         <v>369</v>
       </c>
       <c r="M161" s="0" t="s">
-        <v>448</v>
+        <v>76</v>
       </c>
       <c r="N161" s="0" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="0" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H162" s="0" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I162" s="0" t="s">
         <v>16</v>
@@ -6097,15 +6097,15 @@
         <v>448</v>
       </c>
       <c r="N162" s="0" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="0" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="H163" s="0" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="I163" s="0" t="s">
         <v>16</v>
@@ -6117,15 +6117,15 @@
         <v>448</v>
       </c>
       <c r="N163" s="0" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="0" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="H164" s="0" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I164" s="0" t="s">
         <v>16</v>
@@ -6137,15 +6137,15 @@
         <v>448</v>
       </c>
       <c r="N164" s="0" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="0" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H165" s="0" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I165" s="0" t="s">
         <v>16</v>
@@ -6157,15 +6157,15 @@
         <v>448</v>
       </c>
       <c r="N165" s="0" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="0" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="H166" s="0" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="I166" s="0" t="s">
         <v>16</v>
@@ -6177,15 +6177,15 @@
         <v>448</v>
       </c>
       <c r="N166" s="0" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="0" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H167" s="0" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I167" s="0" t="s">
         <v>16</v>
@@ -6194,18 +6194,18 @@
         <v>369</v>
       </c>
       <c r="M167" s="0" t="s">
-        <v>413</v>
+        <v>448</v>
       </c>
       <c r="N167" s="0" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="0" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H168" s="0" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="I168" s="0" t="s">
         <v>16</v>
@@ -6214,18 +6214,18 @@
         <v>369</v>
       </c>
       <c r="M168" s="0" t="s">
-        <v>154</v>
+        <v>413</v>
       </c>
       <c r="N168" s="0" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="0" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H169" s="0" t="s">
-        <v>435</v>
+        <v>516</v>
       </c>
       <c r="I169" s="0" t="s">
         <v>16</v>
@@ -6237,15 +6237,15 @@
         <v>154</v>
       </c>
       <c r="N169" s="0" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="0" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H170" s="0" t="s">
-        <v>521</v>
+        <v>435</v>
       </c>
       <c r="I170" s="0" t="s">
         <v>16</v>
@@ -6254,18 +6254,18 @@
         <v>369</v>
       </c>
       <c r="M170" s="0" t="s">
-        <v>448</v>
+        <v>154</v>
       </c>
       <c r="N170" s="0" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="0" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="H171" s="0" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="I171" s="0" t="s">
         <v>16</v>
@@ -6277,15 +6277,15 @@
         <v>448</v>
       </c>
       <c r="N171" s="0" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="0" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H172" s="0" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="I172" s="0" t="s">
         <v>16</v>
@@ -6297,15 +6297,15 @@
         <v>448</v>
       </c>
       <c r="N172" s="0" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="0" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H173" s="0" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I173" s="0" t="s">
         <v>16</v>
@@ -6317,15 +6317,15 @@
         <v>448</v>
       </c>
       <c r="N173" s="0" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="0" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="H174" s="0" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="I174" s="0" t="s">
         <v>16</v>
@@ -6337,15 +6337,15 @@
         <v>448</v>
       </c>
       <c r="N174" s="0" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="0" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="H175" s="0" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="I175" s="0" t="s">
         <v>16</v>
@@ -6357,15 +6357,15 @@
         <v>448</v>
       </c>
       <c r="N175" s="0" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="0" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H176" s="0" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="I176" s="0" t="s">
         <v>16</v>
@@ -6377,15 +6377,15 @@
         <v>448</v>
       </c>
       <c r="N176" s="0" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="0" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="H177" s="0" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="I177" s="0" t="s">
         <v>16</v>
@@ -6397,15 +6397,15 @@
         <v>448</v>
       </c>
       <c r="N177" s="0" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="0" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H178" s="0" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I178" s="0" t="s">
         <v>16</v>
@@ -6417,15 +6417,15 @@
         <v>448</v>
       </c>
       <c r="N178" s="0" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="0" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="H179" s="0" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="I179" s="0" t="s">
         <v>16</v>
@@ -6433,19 +6433,19 @@
       <c r="L179" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M179" s="0" t="n">
-        <v>1</v>
+      <c r="M179" s="0" t="s">
+        <v>448</v>
       </c>
       <c r="N179" s="0" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="0" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="H180" s="0" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="I180" s="0" t="s">
         <v>16</v>
@@ -6457,15 +6457,15 @@
         <v>1</v>
       </c>
       <c r="N180" s="0" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="0" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="H181" s="0" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="I181" s="0" t="s">
         <v>16</v>
@@ -6477,15 +6477,15 @@
         <v>1</v>
       </c>
       <c r="N181" s="0" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="0" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="H182" s="0" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="I182" s="0" t="s">
         <v>16</v>
@@ -6497,15 +6497,15 @@
         <v>1</v>
       </c>
       <c r="N182" s="0" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="0" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="H183" s="0" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="I183" s="0" t="s">
         <v>16</v>
@@ -6517,15 +6517,15 @@
         <v>1</v>
       </c>
       <c r="N183" s="0" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="0" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="H184" s="0" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="I184" s="0" t="s">
         <v>16</v>
@@ -6537,15 +6537,15 @@
         <v>1</v>
       </c>
       <c r="N184" s="0" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="0" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="H185" s="0" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="I185" s="0" t="s">
         <v>16</v>
@@ -6553,19 +6553,19 @@
       <c r="L185" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M185" s="0" t="s">
-        <v>35</v>
+      <c r="M185" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N185" s="0" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="0" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="H186" s="0" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="I186" s="0" t="s">
         <v>16</v>
@@ -6577,15 +6577,15 @@
         <v>35</v>
       </c>
       <c r="N186" s="0" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="0" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H187" s="0" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="I187" s="0" t="s">
         <v>16</v>
@@ -6597,15 +6597,15 @@
         <v>35</v>
       </c>
       <c r="N187" s="0" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="0" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="H188" s="0" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="I188" s="0" t="s">
         <v>16</v>
@@ -6622,10 +6622,10 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="0" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H189" s="0" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="I189" s="0" t="s">
         <v>16</v>
@@ -6637,15 +6637,15 @@
         <v>35</v>
       </c>
       <c r="N189" s="0" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="0" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="H190" s="0" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I190" s="0" t="s">
         <v>16</v>
@@ -6657,15 +6657,15 @@
         <v>35</v>
       </c>
       <c r="N190" s="0" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="0" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="H191" s="0" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="I191" s="0" t="s">
         <v>16</v>
@@ -6677,15 +6677,15 @@
         <v>35</v>
       </c>
       <c r="N191" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="0" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H192" s="0" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="I192" s="0" t="s">
         <v>16</v>
@@ -6694,18 +6694,18 @@
         <v>369</v>
       </c>
       <c r="M192" s="0" t="s">
-        <v>413</v>
+        <v>35</v>
       </c>
       <c r="N192" s="0" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="0" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H193" s="0" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="I193" s="0" t="s">
         <v>16</v>
@@ -6717,15 +6717,15 @@
         <v>413</v>
       </c>
       <c r="N193" s="0" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="0" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="H194" s="0" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="I194" s="0" t="s">
         <v>16</v>
@@ -6737,15 +6737,15 @@
         <v>413</v>
       </c>
       <c r="N194" s="0" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="0" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="H195" s="0" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="I195" s="0" t="s">
         <v>16</v>
@@ -6753,19 +6753,19 @@
       <c r="L195" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M195" s="0" t="n">
-        <v>1</v>
+      <c r="M195" s="0" t="s">
+        <v>413</v>
       </c>
       <c r="N195" s="0" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="0" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="H196" s="0" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="I196" s="0" t="s">
         <v>16</v>
@@ -6782,10 +6782,10 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="0" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="H197" s="0" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="I197" s="0" t="s">
         <v>16</v>
@@ -6793,19 +6793,19 @@
       <c r="L197" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M197" s="0" t="s">
-        <v>35</v>
+      <c r="M197" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N197" s="0" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="0" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H198" s="0" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="I198" s="0" t="s">
         <v>16</v>
@@ -6822,10 +6822,10 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="0" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="H199" s="0" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="I199" s="0" t="s">
         <v>16</v>
@@ -6837,15 +6837,15 @@
         <v>35</v>
       </c>
       <c r="N199" s="0" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="0" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="H200" s="0" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I200" s="0" t="s">
         <v>16</v>
@@ -6857,15 +6857,15 @@
         <v>35</v>
       </c>
       <c r="N200" s="0" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="0" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H201" s="0" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="I201" s="0" t="s">
         <v>16</v>
@@ -6877,15 +6877,15 @@
         <v>35</v>
       </c>
       <c r="N201" s="0" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="0" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="H202" s="0" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="I202" s="0" t="s">
         <v>16</v>
@@ -6902,10 +6902,10 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="0" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="H203" s="0" t="s">
-        <v>598</v>
+        <v>612</v>
       </c>
       <c r="I203" s="0" t="s">
         <v>16</v>
@@ -6917,15 +6917,15 @@
         <v>35</v>
       </c>
       <c r="N203" s="0" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="0" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="H204" s="0" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="I204" s="0" t="s">
         <v>16</v>
@@ -6937,15 +6937,15 @@
         <v>35</v>
       </c>
       <c r="N204" s="0" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="0" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H205" s="0" t="s">
-        <v>618</v>
+        <v>601</v>
       </c>
       <c r="I205" s="0" t="s">
         <v>16</v>
@@ -6957,15 +6957,15 @@
         <v>35</v>
       </c>
       <c r="N205" s="0" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="0" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="H206" s="0" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I206" s="0" t="s">
         <v>16</v>
@@ -6982,10 +6982,10 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="0" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="H207" s="0" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="I207" s="0" t="s">
         <v>16</v>
@@ -6994,18 +6994,18 @@
         <v>369</v>
       </c>
       <c r="M207" s="0" t="s">
-        <v>413</v>
+        <v>35</v>
       </c>
       <c r="N207" s="0" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="0" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="H208" s="0" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="I208" s="0" t="s">
         <v>16</v>
@@ -7014,18 +7014,18 @@
         <v>369</v>
       </c>
       <c r="M208" s="0" t="s">
-        <v>35</v>
+        <v>413</v>
       </c>
       <c r="N208" s="0" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="0" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="H209" s="0" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="I209" s="0" t="s">
         <v>16</v>
@@ -7042,10 +7042,10 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="0" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="H210" s="0" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="I210" s="0" t="s">
         <v>16</v>
@@ -7054,18 +7054,18 @@
         <v>369</v>
       </c>
       <c r="M210" s="0" t="s">
-        <v>413</v>
+        <v>35</v>
       </c>
       <c r="N210" s="0" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B211" s="0" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="H211" s="0" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="I211" s="0" t="s">
         <v>16</v>
@@ -7077,15 +7077,15 @@
         <v>413</v>
       </c>
       <c r="N211" s="0" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="0" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="H212" s="0" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="I212" s="0" t="s">
         <v>16</v>
@@ -7097,15 +7097,15 @@
         <v>413</v>
       </c>
       <c r="N212" s="0" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="0" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="H213" s="0" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="I213" s="0" t="s">
         <v>16</v>
@@ -7117,15 +7117,15 @@
         <v>413</v>
       </c>
       <c r="N213" s="0" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="0" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="H214" s="0" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="I214" s="0" t="s">
         <v>16</v>
@@ -7137,15 +7137,15 @@
         <v>413</v>
       </c>
       <c r="N214" s="0" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="0" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H215" s="0" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="I215" s="0" t="s">
         <v>16</v>
@@ -7154,18 +7154,18 @@
         <v>369</v>
       </c>
       <c r="M215" s="0" t="s">
-        <v>35</v>
+        <v>413</v>
       </c>
       <c r="N215" s="0" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="0" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="H216" s="0" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="I216" s="0" t="s">
         <v>16</v>
@@ -7182,10 +7182,10 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="0" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="H217" s="0" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="I217" s="0" t="s">
         <v>16</v>
@@ -7194,18 +7194,18 @@
         <v>369</v>
       </c>
       <c r="M217" s="0" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="N217" s="0" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="0" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="H218" s="0" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="I218" s="0" t="s">
         <v>16</v>
@@ -7214,18 +7214,18 @@
         <v>369</v>
       </c>
       <c r="M218" s="0" t="s">
-        <v>35</v>
+        <v>219</v>
       </c>
       <c r="N218" s="0" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="0" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="H219" s="0" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="I219" s="0" t="s">
         <v>16</v>
@@ -7237,15 +7237,15 @@
         <v>35</v>
       </c>
       <c r="N219" s="0" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="0" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="H220" s="0" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="I220" s="0" t="s">
         <v>16</v>
@@ -7257,15 +7257,15 @@
         <v>35</v>
       </c>
       <c r="N220" s="0" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="0" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="H221" s="0" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="I221" s="0" t="s">
         <v>16</v>
@@ -7277,15 +7277,15 @@
         <v>35</v>
       </c>
       <c r="N221" s="0" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="0" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="H222" s="0" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="I222" s="0" t="s">
         <v>16</v>
@@ -7297,15 +7297,15 @@
         <v>35</v>
       </c>
       <c r="N222" s="0" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="0" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="H223" s="0" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="I223" s="0" t="s">
         <v>16</v>
@@ -7317,15 +7317,15 @@
         <v>35</v>
       </c>
       <c r="N223" s="0" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="0" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="H224" s="0" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="I224" s="0" t="s">
         <v>16</v>
@@ -7337,15 +7337,15 @@
         <v>35</v>
       </c>
       <c r="N224" s="0" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="0" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="H225" s="0" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="I225" s="0" t="s">
         <v>16</v>
@@ -7354,18 +7354,18 @@
         <v>369</v>
       </c>
       <c r="M225" s="0" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N225" s="0" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="0" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="H226" s="0" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="I226" s="0" t="s">
         <v>16</v>
@@ -7377,15 +7377,15 @@
         <v>35</v>
       </c>
       <c r="N226" s="0" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="0" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="H227" s="0" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="I227" s="0" t="s">
         <v>16</v>
@@ -7394,58 +7394,58 @@
         <v>369</v>
       </c>
       <c r="M227" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="N227" s="0" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="0" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="H228" s="0" t="s">
-        <v>680</v>
+        <v>667</v>
       </c>
       <c r="I228" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L228" s="0" t="s">
-        <v>681</v>
+        <v>369</v>
       </c>
       <c r="M228" s="0" t="s">
-        <v>682</v>
+        <v>35</v>
       </c>
       <c r="N228" s="0" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="0" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="H229" s="0" t="s">
-        <v>685</v>
+        <v>670</v>
       </c>
       <c r="I229" s="0" t="s">
         <v>16</v>
       </c>
       <c r="L229" s="0" t="s">
-        <v>681</v>
+        <v>369</v>
       </c>
       <c r="M229" s="0" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="N229" s="0" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="0" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="H230" s="0" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="I230" s="0" t="s">
         <v>16</v>
@@ -7454,18 +7454,18 @@
         <v>681</v>
       </c>
       <c r="M230" s="0" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="N230" s="0" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="0" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="H231" s="0" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="I231" s="0" t="s">
         <v>16</v>
@@ -7474,18 +7474,18 @@
         <v>681</v>
       </c>
       <c r="M231" s="0" t="s">
-        <v>689</v>
+        <v>46</v>
       </c>
       <c r="N231" s="0" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="0" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="H232" s="0" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="I232" s="0" t="s">
         <v>16</v>
@@ -7494,18 +7494,18 @@
         <v>681</v>
       </c>
       <c r="M232" s="0" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="N232" s="0" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="0" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="H233" s="0" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="I233" s="0" t="s">
         <v>16</v>
@@ -7514,18 +7514,18 @@
         <v>681</v>
       </c>
       <c r="M233" s="0" t="s">
-        <v>240</v>
+        <v>689</v>
       </c>
       <c r="N233" s="0" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="0" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="H234" s="0" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="I234" s="0" t="s">
         <v>16</v>
@@ -7534,18 +7534,18 @@
         <v>681</v>
       </c>
       <c r="M234" s="0" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="N234" s="0" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="0" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="H235" s="0" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="I235" s="0" t="s">
         <v>16</v>
@@ -7554,18 +7554,18 @@
         <v>681</v>
       </c>
       <c r="M235" s="0" t="s">
-        <v>703</v>
+        <v>240</v>
       </c>
       <c r="N235" s="0" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="0" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="H236" s="0" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="I236" s="0" t="s">
         <v>16</v>
@@ -7577,15 +7577,15 @@
         <v>703</v>
       </c>
       <c r="N236" s="0" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="0" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="H237" s="0" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="I237" s="0" t="s">
         <v>16</v>
@@ -7594,18 +7594,18 @@
         <v>681</v>
       </c>
       <c r="M237" s="0" t="s">
-        <v>76</v>
+        <v>703</v>
       </c>
       <c r="N237" s="0" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="0" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="H238" s="0" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="I238" s="0" t="s">
         <v>16</v>
@@ -7614,18 +7614,18 @@
         <v>681</v>
       </c>
       <c r="M238" s="0" t="s">
-        <v>76</v>
+        <v>703</v>
       </c>
       <c r="N238" s="0" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="0" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="H239" s="0" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="I239" s="0" t="s">
         <v>16</v>
@@ -7637,15 +7637,15 @@
         <v>76</v>
       </c>
       <c r="N239" s="0" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="0" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="H240" s="0" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="I240" s="0" t="s">
         <v>16</v>
@@ -7657,15 +7657,15 @@
         <v>76</v>
       </c>
       <c r="N240" s="0" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="0" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="H241" s="0" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="I241" s="0" t="s">
         <v>16</v>
@@ -7677,15 +7677,15 @@
         <v>76</v>
       </c>
       <c r="N241" s="0" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="0" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="H242" s="0" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="I242" s="0" t="s">
         <v>16</v>
@@ -7697,15 +7697,15 @@
         <v>76</v>
       </c>
       <c r="N242" s="0" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="0" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="H243" s="0" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="I243" s="0" t="s">
         <v>16</v>
@@ -7717,15 +7717,15 @@
         <v>76</v>
       </c>
       <c r="N243" s="0" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="0" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="H244" s="0" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="I244" s="0" t="s">
         <v>16</v>
@@ -7737,15 +7737,15 @@
         <v>76</v>
       </c>
       <c r="N244" s="0" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="0" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="H245" s="0" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="I245" s="0" t="s">
         <v>16</v>
@@ -7754,18 +7754,18 @@
         <v>681</v>
       </c>
       <c r="M245" s="0" t="s">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="N245" s="0" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="0" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="H246" s="0" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="I246" s="0" t="s">
         <v>16</v>
@@ -7774,18 +7774,18 @@
         <v>681</v>
       </c>
       <c r="M246" s="0" t="s">
-        <v>162</v>
+        <v>76</v>
       </c>
       <c r="N246" s="0" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="0" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="H247" s="0" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="I247" s="0" t="s">
         <v>16</v>
@@ -7794,18 +7794,18 @@
         <v>681</v>
       </c>
       <c r="M247" s="0" t="s">
-        <v>689</v>
+        <v>162</v>
       </c>
       <c r="N247" s="0" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="0" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="H248" s="0" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="I248" s="0" t="s">
         <v>16</v>
@@ -7814,18 +7814,18 @@
         <v>681</v>
       </c>
       <c r="M248" s="0" t="s">
-        <v>689</v>
+        <v>162</v>
       </c>
       <c r="N248" s="0" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="0" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="H249" s="0" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="I249" s="0" t="s">
         <v>16</v>
@@ -7834,18 +7834,18 @@
         <v>681</v>
       </c>
       <c r="M249" s="0" t="s">
-        <v>42</v>
+        <v>689</v>
       </c>
       <c r="N249" s="0" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="0" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="H250" s="0" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="I250" s="0" t="s">
         <v>16</v>
@@ -7854,18 +7854,18 @@
         <v>681</v>
       </c>
       <c r="M250" s="0" t="s">
-        <v>69</v>
+        <v>689</v>
       </c>
       <c r="N250" s="0" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="0" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="H251" s="0" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="I251" s="0" t="s">
         <v>16</v>
@@ -7874,18 +7874,18 @@
         <v>681</v>
       </c>
       <c r="M251" s="0" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="N251" s="0" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="0" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="H252" s="0" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="I252" s="0" t="s">
         <v>16</v>
@@ -7894,18 +7894,18 @@
         <v>681</v>
       </c>
       <c r="M252" s="0" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N252" s="0" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="0" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="H253" s="0" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="I253" s="0" t="s">
         <v>16</v>
@@ -7914,18 +7914,18 @@
         <v>681</v>
       </c>
       <c r="M253" s="0" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N253" s="0" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="0" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="H254" s="0" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="I254" s="0" t="s">
         <v>16</v>
@@ -7934,18 +7934,18 @@
         <v>681</v>
       </c>
       <c r="M254" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="N254" s="0" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="0" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="H255" s="0" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="I255" s="0" t="s">
         <v>16</v>
@@ -7954,18 +7954,18 @@
         <v>681</v>
       </c>
       <c r="M255" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="N255" s="0" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="0" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="H256" s="0" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="I256" s="0" t="s">
         <v>16</v>
@@ -7974,18 +7974,18 @@
         <v>681</v>
       </c>
       <c r="M256" s="0" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="N256" s="0" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="0" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="H257" s="0" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="I257" s="0" t="s">
         <v>16</v>
@@ -7994,18 +7994,18 @@
         <v>681</v>
       </c>
       <c r="M257" s="0" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="N257" s="0" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="0" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="H258" s="0" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="I258" s="0" t="s">
         <v>16</v>
@@ -8017,15 +8017,15 @@
         <v>280</v>
       </c>
       <c r="N258" s="0" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="0" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="H259" s="0" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="I259" s="0" t="s">
         <v>16</v>
@@ -8037,15 +8037,15 @@
         <v>280</v>
       </c>
       <c r="N259" s="0" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="0" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="H260" s="0" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="I260" s="0" t="s">
         <v>16</v>
@@ -8057,15 +8057,15 @@
         <v>280</v>
       </c>
       <c r="N260" s="0" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="0" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="H261" s="0" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="I261" s="0" t="s">
         <v>16</v>
@@ -8077,15 +8077,15 @@
         <v>280</v>
       </c>
       <c r="N261" s="0" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="0" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="H262" s="0" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="I262" s="0" t="s">
         <v>16</v>
@@ -8094,18 +8094,18 @@
         <v>681</v>
       </c>
       <c r="M262" s="0" t="s">
-        <v>788</v>
+        <v>280</v>
       </c>
       <c r="N262" s="0" t="s">
-        <v>789</v>
+        <v>782</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="0" t="s">
-        <v>790</v>
+        <v>783</v>
       </c>
       <c r="H263" s="0" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
       <c r="I263" s="0" t="s">
         <v>16</v>
@@ -8114,18 +8114,18 @@
         <v>681</v>
       </c>
       <c r="M263" s="0" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="N263" s="0" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="0" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="H264" s="0" t="s">
-        <v>794</v>
+        <v>787</v>
       </c>
       <c r="I264" s="0" t="s">
         <v>16</v>
@@ -8134,18 +8134,18 @@
         <v>681</v>
       </c>
       <c r="M264" s="0" t="s">
-        <v>42</v>
+        <v>788</v>
       </c>
       <c r="N264" s="0" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="0" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="H265" s="0" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="I265" s="0" t="s">
         <v>16</v>
@@ -8154,18 +8154,18 @@
         <v>681</v>
       </c>
       <c r="M265" s="0" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="N265" s="0" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="0" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="H266" s="0" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="I266" s="0" t="s">
         <v>16</v>
@@ -8174,18 +8174,18 @@
         <v>681</v>
       </c>
       <c r="M266" s="0" t="s">
-        <v>154</v>
+        <v>42</v>
       </c>
       <c r="N266" s="0" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="0" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
       <c r="H267" s="0" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="I267" s="0" t="s">
         <v>16</v>
@@ -8194,18 +8194,18 @@
         <v>681</v>
       </c>
       <c r="M267" s="0" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="N267" s="0" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="0" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
       <c r="H268" s="0" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="I268" s="0" t="s">
         <v>16</v>
@@ -8213,19 +8213,19 @@
       <c r="L268" s="0" t="s">
         <v>681</v>
       </c>
-      <c r="M268" s="0" t="n">
-        <v>0.001</v>
+      <c r="M268" s="0" t="s">
+        <v>154</v>
       </c>
       <c r="N268" s="0" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="0" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="H269" s="0" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="I269" s="0" t="s">
         <v>16</v>
@@ -8234,18 +8234,18 @@
         <v>681</v>
       </c>
       <c r="M269" s="0" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="N269" s="0" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="0" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="H270" s="0" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="I270" s="0" t="s">
         <v>16</v>
@@ -8253,19 +8253,19 @@
       <c r="L270" s="0" t="s">
         <v>681</v>
       </c>
-      <c r="M270" s="0" t="s">
-        <v>703</v>
+      <c r="M270" s="0" t="n">
+        <v>0.001</v>
       </c>
       <c r="N270" s="0" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="0" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="H271" s="0" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="I271" s="0" t="s">
         <v>16</v>
@@ -8274,18 +8274,18 @@
         <v>681</v>
       </c>
       <c r="M271" s="0" t="s">
-        <v>788</v>
+        <v>154</v>
       </c>
       <c r="N271" s="0" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="0" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="H272" s="0" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="I272" s="0" t="s">
         <v>16</v>
@@ -8294,18 +8294,18 @@
         <v>681</v>
       </c>
       <c r="M272" s="0" t="s">
-        <v>154</v>
+        <v>703</v>
       </c>
       <c r="N272" s="0" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="0" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="H273" s="0" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="I273" s="0" t="s">
         <v>16</v>
@@ -8314,18 +8314,18 @@
         <v>681</v>
       </c>
       <c r="M273" s="0" t="s">
-        <v>42</v>
+        <v>788</v>
       </c>
       <c r="N273" s="0" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="0" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="H274" s="0" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="I274" s="0" t="s">
         <v>16</v>
@@ -8334,18 +8334,18 @@
         <v>681</v>
       </c>
       <c r="M274" s="0" t="s">
-        <v>330</v>
+        <v>154</v>
       </c>
       <c r="N274" s="0" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="0" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="H275" s="0" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="I275" s="0" t="s">
         <v>16</v>
@@ -8354,18 +8354,18 @@
         <v>681</v>
       </c>
       <c r="M275" s="0" t="s">
-        <v>696</v>
+        <v>42</v>
       </c>
       <c r="N275" s="0" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="0" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="H276" s="0" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="I276" s="0" t="s">
         <v>16</v>
@@ -8374,18 +8374,18 @@
         <v>681</v>
       </c>
       <c r="M276" s="0" t="s">
-        <v>696</v>
+        <v>330</v>
       </c>
       <c r="N276" s="0" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="0" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="H277" s="0" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="I277" s="0" t="s">
         <v>16</v>
@@ -8394,18 +8394,18 @@
         <v>681</v>
       </c>
       <c r="M277" s="0" t="s">
-        <v>280</v>
+        <v>696</v>
       </c>
       <c r="N277" s="0" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="0" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="H278" s="0" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="I278" s="0" t="s">
         <v>16</v>
@@ -8414,18 +8414,18 @@
         <v>681</v>
       </c>
       <c r="M278" s="0" t="s">
-        <v>280</v>
+        <v>696</v>
       </c>
       <c r="N278" s="0" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="0" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="H279" s="0" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="I279" s="0" t="s">
         <v>16</v>
@@ -8437,15 +8437,15 @@
         <v>280</v>
       </c>
       <c r="N279" s="0" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="0" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="H280" s="0" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="I280" s="0" t="s">
         <v>16</v>
@@ -8457,15 +8457,15 @@
         <v>280</v>
       </c>
       <c r="N280" s="0" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="0" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="H281" s="0" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="I281" s="0" t="s">
         <v>16</v>
@@ -8474,18 +8474,18 @@
         <v>681</v>
       </c>
       <c r="M281" s="0" t="s">
-        <v>846</v>
+        <v>280</v>
       </c>
       <c r="N281" s="0" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="0" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="H282" s="0" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="I282" s="0" t="s">
         <v>16</v>
@@ -8494,18 +8494,18 @@
         <v>681</v>
       </c>
       <c r="M282" s="0" t="s">
-        <v>846</v>
+        <v>280</v>
       </c>
       <c r="N282" s="0" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="0" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="H283" s="0" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="I283" s="0" t="s">
         <v>16</v>
@@ -8517,15 +8517,15 @@
         <v>846</v>
       </c>
       <c r="N283" s="0" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="0" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="H284" s="0" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="I284" s="0" t="s">
         <v>16</v>
@@ -8534,18 +8534,18 @@
         <v>681</v>
       </c>
       <c r="M284" s="0" t="s">
-        <v>42</v>
+        <v>846</v>
       </c>
       <c r="N284" s="0" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="0" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="H285" s="0" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="I285" s="0" t="s">
         <v>16</v>
@@ -8553,19 +8553,19 @@
       <c r="L285" s="0" t="s">
         <v>681</v>
       </c>
-      <c r="M285" s="0" t="n">
-        <v>1</v>
+      <c r="M285" s="0" t="s">
+        <v>846</v>
       </c>
       <c r="N285" s="0" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="0" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="H286" s="0" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="I286" s="0" t="s">
         <v>16</v>
@@ -8574,18 +8574,18 @@
         <v>681</v>
       </c>
       <c r="M286" s="0" t="s">
-        <v>330</v>
+        <v>42</v>
       </c>
       <c r="N286" s="0" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="0" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="H287" s="0" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="I287" s="0" t="s">
         <v>16</v>
@@ -8593,19 +8593,19 @@
       <c r="L287" s="0" t="s">
         <v>681</v>
       </c>
-      <c r="M287" s="0" t="s">
-        <v>330</v>
+      <c r="M287" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N287" s="0" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="0" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="H288" s="0" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="I288" s="0" t="s">
         <v>16</v>
@@ -8614,18 +8614,18 @@
         <v>681</v>
       </c>
       <c r="M288" s="0" t="s">
-        <v>42</v>
+        <v>330</v>
       </c>
       <c r="N288" s="0" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B289" s="0" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="H289" s="0" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="I289" s="0" t="s">
         <v>16</v>
@@ -8634,18 +8634,18 @@
         <v>681</v>
       </c>
       <c r="M289" s="0" t="s">
-        <v>871</v>
+        <v>330</v>
       </c>
       <c r="N289" s="0" t="s">
-        <v>872</v>
+        <v>865</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="0" t="s">
-        <v>873</v>
+        <v>866</v>
       </c>
       <c r="H290" s="0" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
       <c r="I290" s="0" t="s">
         <v>16</v>
@@ -8654,18 +8654,18 @@
         <v>681</v>
       </c>
       <c r="M290" s="0" t="s">
-        <v>871</v>
+        <v>42</v>
       </c>
       <c r="N290" s="0" t="s">
-        <v>875</v>
+        <v>868</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="0" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="H291" s="0" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
       <c r="I291" s="0" t="s">
         <v>16</v>
@@ -8674,18 +8674,18 @@
         <v>681</v>
       </c>
       <c r="M291" s="0" t="s">
-        <v>76</v>
+        <v>871</v>
       </c>
       <c r="N291" s="0" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B292" s="0" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="H292" s="0" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="I292" s="0" t="s">
         <v>16</v>
@@ -8694,18 +8694,18 @@
         <v>681</v>
       </c>
       <c r="M292" s="0" t="s">
-        <v>76</v>
+        <v>871</v>
       </c>
       <c r="N292" s="0" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="0" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="H293" s="0" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="I293" s="0" t="s">
         <v>16</v>
@@ -8717,15 +8717,15 @@
         <v>76</v>
       </c>
       <c r="N293" s="0" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B294" s="0" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="H294" s="0" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="I294" s="0" t="s">
         <v>16</v>
@@ -8737,15 +8737,15 @@
         <v>76</v>
       </c>
       <c r="N294" s="0" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B295" s="0" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="H295" s="0" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="I295" s="0" t="s">
         <v>16</v>
@@ -8757,15 +8757,15 @@
         <v>76</v>
       </c>
       <c r="N295" s="0" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="0" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="H296" s="0" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="I296" s="0" t="s">
         <v>16</v>
@@ -8774,9 +8774,49 @@
         <v>681</v>
       </c>
       <c r="M296" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N296" s="0" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B297" s="0" t="s">
+        <v>888</v>
+      </c>
+      <c r="H297" s="0" t="s">
+        <v>889</v>
+      </c>
+      <c r="I297" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L297" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="M297" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N297" s="0" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B298" s="0" t="s">
+        <v>891</v>
+      </c>
+      <c r="H298" s="0" t="s">
+        <v>892</v>
+      </c>
+      <c r="I298" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L298" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="M298" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="N296" s="0" t="s">
+      <c r="N298" s="0" t="s">
         <v>893</v>
       </c>
     </row>

</xml_diff>